<commit_message>
Descripciones de algunos recursos ampliadas
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion01/ESCALETA_CN_09_01_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion01/ESCALETA_CN_09_01_CO.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="247">
   <si>
     <t>Asignatura</t>
   </si>
@@ -347,9 +347,6 @@
     <t>Interactivo que presenta las principales moléculas involucradas en la herencia y la síntesis de proteínas</t>
   </si>
   <si>
-    <t xml:space="preserve">Cada pestaña es un tipo de molécula. Se presentan el ADN y el ARN (en dos pestañas aparte) aclarando que ambas moléculas son ácidos nucléicos y presentando los nucleótidos. Luego se presentan las proteínas, y se explica que se conforman de aminoácidos. Recordar explicar las moléculas de manera sencilla, sin olvidar que los estudiantes de este curso no han visto química orgánica. </t>
-  </si>
-  <si>
     <t>El ADN</t>
   </si>
   <si>
@@ -371,9 +368,6 @@
     <t>Actividad que permite reconocer las diferencias entre el ARN y el ADN</t>
   </si>
   <si>
-    <t>Ver anotaciones en guion</t>
-  </si>
-  <si>
     <t>Las proteínas</t>
   </si>
   <si>
@@ -608,9 +602,6 @@
     <t>Recurso M5B-01</t>
   </si>
   <si>
-    <t>Recurso M1B-02</t>
-  </si>
-  <si>
     <t>4º ESO</t>
   </si>
   <si>
@@ -711,6 +702,68 @@
   </si>
   <si>
     <t>Mapa conceptual</t>
+  </si>
+  <si>
+    <t>Preguntas sobre la historia d ela biología molecular y sobre el "dogma central" de la biología molecular. Hay propuestas de preguntas en el cuaderno de estudio.</t>
+  </si>
+  <si>
+    <t>Preguntas varias sobre las moléculas de la herencia. Hay propuestas de preguntas en el cuaderno de estudio.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se propone que  un contenedor con el término ADN, en donde se ubucan las palabras: Desoxinucleótidos, desoxirribosa, A T C G, doble cadena. El contenedor 2 es ARN e incluye los
+términos: Ribonucleótido, ribosa, A U C G, cadena sencilla. Proponer más términos, pero cuidando que no apliquen para ambos tipos de molécula. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asociar 1 sonido 1 texto (M3B). Los audios contienen descripciones y los textos el término descrito. Por ejemplo: Audio “moléculas pequeñas compuestas principalmente por carbono, hidrógeno, oxígeno y nitrógeno” y el texto asociado es “Aminoácidos”. </t>
+  </si>
+  <si>
+    <t>Cada pestaña es un tipo de molécula. Se presentan el ADN y el ARN (en dos pestañas aparte) aclarando que ambas moléculas son ácidos nucléicos y presentando los nucleótidos. Luego se presentan las proteínas, y se explica que se conforman de aminoácidos. Recordar explicar las moléculas de manera sencilla, sin olvidar que los estudiantes de este curso no han visto química orgánica.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se propone aquí una actividad de posicionar etiquetas en imagen (M9B) en la cual se presenta la estructura del ADN y allí los estudiantes reconocen: el azúcar, la base nitrogenada (Adenina, Timina, Citocina, Guanina), el fosfato, puentes de hidrógeno.
+</t>
+  </si>
+  <si>
+    <t>Se hace un video que muestre el proceso de replicación del ADN</t>
+  </si>
+  <si>
+    <t>Se escribe el proceso de replicación del ADN es frases cortas, para que el estudiante ordene según la secuancia en la que se da cada paso descrito.</t>
+  </si>
+  <si>
+    <t>Recurso M12A-02</t>
+  </si>
+  <si>
+    <t>Preguntas sobre replicación del ADN y mutaciones.</t>
+  </si>
+  <si>
+    <t>Se hace un video que muestre el proceso de transcripción del ADN</t>
+  </si>
+  <si>
+    <t>Se hace un video que muestre el proceso de traducción del ADN</t>
+  </si>
+  <si>
+    <t>Los estudiantes ordenan la secuencia de eventos ocurridos durante la traducción.</t>
+  </si>
+  <si>
+    <t>Los estudiantes asocian el significado correspondiente, con los siguientes términos: cáncer, apoptosis, metástasis, oncogen, ciclo celular, mutación</t>
+  </si>
+  <si>
+    <t>Los estudiantes completan oraciones acerca de la transcripción el ADN</t>
+  </si>
+  <si>
+    <t>Las preguntas deben tener las siguientes opciones de respuesta (que son las palabras del juego): ADN, ARN, proteína, enzima, nucleótido, aminoácido, base nitrogenada, uracilo.</t>
+  </si>
+  <si>
+    <t>Preguntas sobre el cáncer. Se puede preguntar qué es, si es heredable, cómo se relaciona con la información genética, qué relación tiene con la transcripción, la traducción o la replicación.</t>
+  </si>
+  <si>
+    <t>Actividad grupal en la cual se otorgan moldes de desoxirribosa, fosfato y bases nitrogenadas del ADN. Cada estudiante los imprime, obtiene copias, recorta y arma los cuatro desoxinucleótidos. Con dicho insumo, entre todo el grupo arman una gran molécula de ADN. Una vez esto, escriben la secuencia obtenida y realizan el ejercicio teórico de transcripción y de traducción de dicha secuencia.</t>
+  </si>
+  <si>
+    <t>Actividad en la que se otorgan dos secuencias reales de ADN, una normal y una mutada; por ejemplo de la anemia falciforme. Los estudiantes comparan las secuencias e identifican la mutación, además realizan la transcripción y la traducción de cada secuencia y reconocen la manera en la que el cambio de los nucleótidos afecta la proteína. También realizan una búsqueda de información acerca de la condición y sus afectaciones moleculares.</t>
+  </si>
+  <si>
+    <t>Por grupos, los estudiantes eligen algún tipo de cáncer, realizan una búsqueda de información guiada por el docente, y con esta organizan una exposición basada en la información molecular de la enfermedad, la cual presentan al resto de la clase.</t>
   </si>
 </sst>
 </file>
@@ -1639,7 +1692,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1647,10 +1700,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U36"/>
+  <dimension ref="A1:U37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection sqref="A1:A2"/>
+    <sheetView tabSelected="1" topLeftCell="K8" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="O35" sqref="O35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1784,10 +1837,10 @@
       </c>
       <c r="E3" s="30"/>
       <c r="F3" s="52" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="G3" s="54" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="H3" s="31">
         <v>1</v>
@@ -1818,16 +1871,16 @@
         <v>6</v>
       </c>
       <c r="R3" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="S3" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="T3" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="S3" s="19" t="s">
+      <c r="U3" s="20" t="s">
         <v>164</v>
-      </c>
-      <c r="T3" s="19" t="s">
-        <v>165</v>
-      </c>
-      <c r="U3" s="20" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1848,7 +1901,7 @@
       </c>
       <c r="F4" s="35"/>
       <c r="G4" s="56" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="H4" s="27">
         <v>2</v>
@@ -1857,7 +1910,7 @@
         <v>92</v>
       </c>
       <c r="J4" s="45" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="K4" s="46" t="s">
         <v>69</v>
@@ -1870,7 +1923,7 @@
         <v>62</v>
       </c>
       <c r="O4" s="47" t="s">
-        <v>116</v>
+        <v>227</v>
       </c>
       <c r="P4" s="42" t="s">
         <v>19</v>
@@ -1879,16 +1932,16 @@
         <v>6</v>
       </c>
       <c r="R4" s="50" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="S4" s="50" t="s">
+        <v>172</v>
+      </c>
+      <c r="T4" s="50" t="s">
+        <v>175</v>
+      </c>
+      <c r="U4" s="51" t="s">
         <v>174</v>
-      </c>
-      <c r="T4" s="50" t="s">
-        <v>177</v>
-      </c>
-      <c r="U4" s="51" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1929,7 +1982,7 @@
       </c>
       <c r="N5" s="9"/>
       <c r="O5" s="8" t="s">
-        <v>108</v>
+        <v>231</v>
       </c>
       <c r="P5" s="42" t="s">
         <v>19</v>
@@ -1938,16 +1991,16 @@
         <v>6</v>
       </c>
       <c r="R5" s="11" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="S5" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="T5" s="41" t="s">
+        <v>168</v>
+      </c>
+      <c r="U5" s="1" t="s">
         <v>164</v>
-      </c>
-      <c r="T5" s="41" t="s">
-        <v>170</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1988,7 +2041,7 @@
         <v>23</v>
       </c>
       <c r="O6" s="47" t="s">
-        <v>116</v>
+        <v>228</v>
       </c>
       <c r="P6" s="62" t="s">
         <v>19</v>
@@ -1997,16 +2050,16 @@
         <v>6</v>
       </c>
       <c r="R6" s="11" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="S6" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="T6" s="41" t="s">
+        <v>183</v>
+      </c>
+      <c r="U6" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="T6" s="41" t="s">
-        <v>185</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2026,10 +2079,10 @@
         <v>104</v>
       </c>
       <c r="F7" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="G7" s="37" t="s">
         <v>109</v>
-      </c>
-      <c r="G7" s="37" t="s">
-        <v>110</v>
       </c>
       <c r="H7" s="27">
         <v>5</v>
@@ -2038,7 +2091,7 @@
         <v>91</v>
       </c>
       <c r="J7" s="38" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="K7" s="40" t="s">
         <v>70</v>
@@ -2053,19 +2106,19 @@
         <v>19</v>
       </c>
       <c r="Q7" s="59" t="s">
+        <v>193</v>
+      </c>
+      <c r="R7" s="24" t="s">
+        <v>194</v>
+      </c>
+      <c r="S7" s="24" t="s">
+        <v>195</v>
+      </c>
+      <c r="T7" s="24" t="s">
         <v>196</v>
       </c>
-      <c r="R7" s="24" t="s">
+      <c r="U7" s="33" t="s">
         <v>197</v>
-      </c>
-      <c r="S7" s="24" t="s">
-        <v>198</v>
-      </c>
-      <c r="T7" s="24" t="s">
-        <v>199</v>
-      </c>
-      <c r="U7" s="33" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2085,10 +2138,10 @@
         <v>104</v>
       </c>
       <c r="F8" s="35" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G8" s="37" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H8" s="27">
         <v>6</v>
@@ -2097,7 +2150,7 @@
         <v>92</v>
       </c>
       <c r="J8" s="38" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K8" s="40" t="s">
         <v>69</v>
@@ -2110,7 +2163,7 @@
         <v>50</v>
       </c>
       <c r="O8" s="47" t="s">
-        <v>116</v>
+        <v>232</v>
       </c>
       <c r="P8" s="63" t="s">
         <v>19</v>
@@ -2119,16 +2172,16 @@
         <v>6</v>
       </c>
       <c r="R8" s="24" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="S8" s="24" t="s">
+        <v>172</v>
+      </c>
+      <c r="T8" s="24" t="s">
+        <v>186</v>
+      </c>
+      <c r="U8" s="33" t="s">
         <v>174</v>
-      </c>
-      <c r="T8" s="24" t="s">
-        <v>188</v>
-      </c>
-      <c r="U8" s="33" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2148,10 +2201,10 @@
         <v>104</v>
       </c>
       <c r="F9" s="35" t="s">
+        <v>112</v>
+      </c>
+      <c r="G9" s="57" t="s">
         <v>113</v>
-      </c>
-      <c r="G9" s="57" t="s">
-        <v>114</v>
       </c>
       <c r="H9" s="27">
         <v>7</v>
@@ -2160,7 +2213,7 @@
         <v>92</v>
       </c>
       <c r="J9" s="38" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K9" s="40" t="s">
         <v>69</v>
@@ -2173,7 +2226,7 @@
         <v>24</v>
       </c>
       <c r="O9" s="47" t="s">
-        <v>116</v>
+        <v>229</v>
       </c>
       <c r="P9" s="63" t="s">
         <v>19</v>
@@ -2182,16 +2235,16 @@
         <v>6</v>
       </c>
       <c r="R9" s="24" t="s">
+        <v>171</v>
+      </c>
+      <c r="S9" s="24" t="s">
+        <v>172</v>
+      </c>
+      <c r="T9" s="24" t="s">
         <v>173</v>
       </c>
-      <c r="S9" s="24" t="s">
+      <c r="U9" s="33" t="s">
         <v>174</v>
-      </c>
-      <c r="T9" s="24" t="s">
-        <v>175</v>
-      </c>
-      <c r="U9" s="33" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2208,13 +2261,13 @@
         <v>101</v>
       </c>
       <c r="E10" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="F10" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="G10" s="56" t="s">
         <v>117</v>
-      </c>
-      <c r="F10" s="35" t="s">
-        <v>118</v>
-      </c>
-      <c r="G10" s="56" t="s">
-        <v>119</v>
       </c>
       <c r="H10" s="27">
         <v>8</v>
@@ -2223,7 +2276,7 @@
         <v>92</v>
       </c>
       <c r="J10" s="38" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="K10" s="40" t="s">
         <v>69</v>
@@ -2236,7 +2289,7 @@
         <v>79</v>
       </c>
       <c r="O10" s="47" t="s">
-        <v>116</v>
+        <v>230</v>
       </c>
       <c r="P10" s="63" t="s">
         <v>19</v>
@@ -2245,16 +2298,16 @@
         <v>6</v>
       </c>
       <c r="R10" s="11" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="S10" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="T10" s="41" t="s">
+        <v>187</v>
+      </c>
+      <c r="U10" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="T10" s="41" t="s">
-        <v>189</v>
-      </c>
-      <c r="U10" s="1" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2271,13 +2324,13 @@
         <v>101</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F11" s="35" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G11" s="58" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="H11" s="27">
         <v>9</v>
@@ -2286,7 +2339,7 @@
         <v>92</v>
       </c>
       <c r="J11" s="38" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="K11" s="40" t="s">
         <v>69</v>
@@ -2299,7 +2352,7 @@
         <v>61</v>
       </c>
       <c r="O11" s="47" t="s">
-        <v>116</v>
+        <v>242</v>
       </c>
       <c r="P11" s="63" t="s">
         <v>20</v>
@@ -2308,16 +2361,16 @@
         <v>6</v>
       </c>
       <c r="R11" s="24" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="S11" s="24" t="s">
+        <v>172</v>
+      </c>
+      <c r="T11" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="U11" s="33" t="s">
         <v>174</v>
-      </c>
-      <c r="T11" s="24" t="s">
-        <v>190</v>
-      </c>
-      <c r="U11" s="33" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2338,7 +2391,7 @@
       </c>
       <c r="F12" s="35"/>
       <c r="G12" s="37" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H12" s="27">
         <v>10</v>
@@ -2347,7 +2400,7 @@
         <v>92</v>
       </c>
       <c r="J12" s="38" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="K12" s="40" t="s">
         <v>69</v>
@@ -2360,7 +2413,7 @@
         <v>62</v>
       </c>
       <c r="O12" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="P12" s="63" t="s">
         <v>19</v>
@@ -2369,16 +2422,16 @@
         <v>6</v>
       </c>
       <c r="R12" s="24" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="S12" s="24" t="s">
+        <v>172</v>
+      </c>
+      <c r="T12" s="24" t="s">
+        <v>176</v>
+      </c>
+      <c r="U12" s="33" t="s">
         <v>174</v>
-      </c>
-      <c r="T12" s="24" t="s">
-        <v>178</v>
-      </c>
-      <c r="U12" s="33" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2392,14 +2445,14 @@
         <v>97</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F13" s="35"/>
       <c r="G13" s="37" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="H13" s="27">
         <v>11</v>
@@ -2408,7 +2461,7 @@
         <v>91</v>
       </c>
       <c r="J13" s="38" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="K13" s="40" t="s">
         <v>69</v>
@@ -2421,7 +2474,7 @@
       </c>
       <c r="N13" s="9"/>
       <c r="O13" s="47" t="s">
-        <v>116</v>
+        <v>233</v>
       </c>
       <c r="P13" s="63" t="s">
         <v>19</v>
@@ -2430,16 +2483,16 @@
         <v>6</v>
       </c>
       <c r="R13" s="25" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="S13" s="25" t="s">
+        <v>162</v>
+      </c>
+      <c r="T13" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="U13" s="34" t="s">
         <v>164</v>
-      </c>
-      <c r="T13" s="25" t="s">
-        <v>167</v>
-      </c>
-      <c r="U13" s="34" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2453,14 +2506,14 @@
         <v>97</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E14" s="26" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F14" s="35"/>
       <c r="G14" s="37" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="H14" s="27">
         <v>12</v>
@@ -2469,7 +2522,7 @@
         <v>92</v>
       </c>
       <c r="J14" s="38" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="K14" s="40" t="s">
         <v>69</v>
@@ -2479,10 +2532,10 @@
       </c>
       <c r="M14" s="9"/>
       <c r="N14" s="9" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="O14" s="47" t="s">
-        <v>116</v>
+        <v>234</v>
       </c>
       <c r="P14" s="63" t="s">
         <v>19</v>
@@ -2491,16 +2544,16 @@
         <v>6</v>
       </c>
       <c r="R14" s="25" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="S14" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="T14" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="U14" s="34" t="s">
         <v>174</v>
-      </c>
-      <c r="T14" s="25" t="s">
-        <v>186</v>
-      </c>
-      <c r="U14" s="34" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2514,14 +2567,14 @@
         <v>97</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E15" s="26" t="s">
         <v>96</v>
       </c>
       <c r="F15" s="35"/>
       <c r="G15" s="37" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H15" s="27">
         <v>13</v>
@@ -2530,7 +2583,7 @@
         <v>91</v>
       </c>
       <c r="J15" s="38" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="K15" s="40" t="s">
         <v>70</v>
@@ -2545,19 +2598,19 @@
         <v>19</v>
       </c>
       <c r="Q15" s="61" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="R15" s="25" t="s">
+        <v>194</v>
+      </c>
+      <c r="S15" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="T15" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="U15" s="34" t="s">
         <v>197</v>
-      </c>
-      <c r="S15" s="25" t="s">
-        <v>198</v>
-      </c>
-      <c r="T15" s="25" t="s">
-        <v>127</v>
-      </c>
-      <c r="U15" s="34" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2571,14 +2624,14 @@
         <v>97</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E16" s="26" t="s">
         <v>96</v>
       </c>
       <c r="F16" s="35"/>
       <c r="G16" s="37" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="H16" s="27">
         <v>14</v>
@@ -2587,7 +2640,7 @@
         <v>92</v>
       </c>
       <c r="J16" s="38" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="K16" s="40" t="s">
         <v>70</v>
@@ -2602,19 +2655,19 @@
         <v>19</v>
       </c>
       <c r="Q16" s="60" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="R16" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="S16" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="T16" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="U16" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="S16" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="T16" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="U16" s="1" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2628,14 +2681,14 @@
         <v>97</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E17" s="26" t="s">
         <v>100</v>
       </c>
       <c r="F17" s="35"/>
       <c r="G17" s="37" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="H17" s="27">
         <v>15</v>
@@ -2644,7 +2697,7 @@
         <v>92</v>
       </c>
       <c r="J17" s="38" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="K17" s="40" t="s">
         <v>69</v>
@@ -2657,7 +2710,7 @@
         <v>62</v>
       </c>
       <c r="O17" s="47" t="s">
-        <v>116</v>
+        <v>236</v>
       </c>
       <c r="P17" s="63" t="s">
         <v>19</v>
@@ -2666,16 +2719,16 @@
         <v>6</v>
       </c>
       <c r="R17" s="11" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="S17" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="T17" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="U17" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="T17" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="U17" s="1" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2689,14 +2742,14 @@
         <v>97</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E18" s="26" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F18" s="35"/>
       <c r="G18" s="37" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H18" s="27">
         <v>16</v>
@@ -2705,7 +2758,7 @@
         <v>91</v>
       </c>
       <c r="J18" s="38" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="K18" s="40" t="s">
         <v>69</v>
@@ -2718,7 +2771,7 @@
       </c>
       <c r="N18" s="9"/>
       <c r="O18" s="47" t="s">
-        <v>116</v>
+        <v>237</v>
       </c>
       <c r="P18" s="63" t="s">
         <v>19</v>
@@ -2727,16 +2780,16 @@
         <v>6</v>
       </c>
       <c r="R18" s="11" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="S18" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="T18" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="U18" s="1" t="s">
         <v>164</v>
-      </c>
-      <c r="T18" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="U18" s="1" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2750,14 +2803,14 @@
         <v>97</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E19" s="26" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F19" s="35"/>
       <c r="G19" s="37" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H19" s="27">
         <v>17</v>
@@ -2766,7 +2819,7 @@
         <v>92</v>
       </c>
       <c r="J19" s="38" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="K19" s="40" t="s">
         <v>69</v>
@@ -2779,7 +2832,7 @@
         <v>22</v>
       </c>
       <c r="O19" s="47" t="s">
-        <v>116</v>
+        <v>241</v>
       </c>
       <c r="P19" s="63" t="s">
         <v>19</v>
@@ -2788,16 +2841,16 @@
         <v>6</v>
       </c>
       <c r="R19" s="11" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="S19" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="T19" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="U19" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="T19" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="U19" s="1" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2811,14 +2864,14 @@
         <v>97</v>
       </c>
       <c r="D20" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="E20" s="26" t="s">
         <v>130</v>
-      </c>
-      <c r="E20" s="26" t="s">
-        <v>132</v>
       </c>
       <c r="F20" s="35"/>
       <c r="G20" s="37" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H20" s="27">
         <v>18</v>
@@ -2827,7 +2880,7 @@
         <v>91</v>
       </c>
       <c r="J20" s="38" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K20" s="40" t="s">
         <v>69</v>
@@ -2840,7 +2893,7 @@
       </c>
       <c r="N20" s="9"/>
       <c r="O20" s="47" t="s">
-        <v>116</v>
+        <v>238</v>
       </c>
       <c r="P20" s="63" t="s">
         <v>19</v>
@@ -2849,16 +2902,16 @@
         <v>6</v>
       </c>
       <c r="R20" s="11" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="S20" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="T20" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="U20" s="1" t="s">
         <v>164</v>
-      </c>
-      <c r="T20" s="11" t="s">
-        <v>169</v>
-      </c>
-      <c r="U20" s="1" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2872,14 +2925,14 @@
         <v>97</v>
       </c>
       <c r="D21" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="E21" s="26" t="s">
         <v>130</v>
-      </c>
-      <c r="E21" s="26" t="s">
-        <v>132</v>
       </c>
       <c r="F21" s="35"/>
       <c r="G21" s="37" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="H21" s="27">
         <v>19</v>
@@ -2888,7 +2941,7 @@
         <v>92</v>
       </c>
       <c r="J21" s="38" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="K21" s="40" t="s">
         <v>70</v>
@@ -2903,19 +2956,19 @@
         <v>19</v>
       </c>
       <c r="Q21" s="61" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="R21" s="25" t="s">
+        <v>194</v>
+      </c>
+      <c r="S21" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="T21" s="25" t="s">
+        <v>199</v>
+      </c>
+      <c r="U21" s="34" t="s">
         <v>197</v>
-      </c>
-      <c r="S21" s="25" t="s">
-        <v>198</v>
-      </c>
-      <c r="T21" s="25" t="s">
-        <v>202</v>
-      </c>
-      <c r="U21" s="34" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2929,16 +2982,16 @@
         <v>97</v>
       </c>
       <c r="D22" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="E22" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="E22" s="26" t="s">
-        <v>132</v>
-      </c>
       <c r="F22" s="35" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G22" s="37" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H22" s="27">
         <v>20</v>
@@ -2947,7 +3000,7 @@
         <v>91</v>
       </c>
       <c r="J22" s="38" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="K22" s="40" t="s">
         <v>69</v>
@@ -2960,7 +3013,7 @@
       </c>
       <c r="N22" s="9"/>
       <c r="O22" s="8" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="P22" s="63" t="s">
         <v>19</v>
@@ -2969,16 +3022,16 @@
         <v>6</v>
       </c>
       <c r="R22" s="25" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="S22" s="25" t="s">
+        <v>162</v>
+      </c>
+      <c r="T22" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="U22" s="34" t="s">
         <v>164</v>
-      </c>
-      <c r="T22" s="25" t="s">
-        <v>171</v>
-      </c>
-      <c r="U22" s="34" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="23" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2992,16 +3045,16 @@
         <v>97</v>
       </c>
       <c r="D23" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="E23" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="E23" s="26" t="s">
-        <v>132</v>
-      </c>
       <c r="F23" s="35" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G23" s="37" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H23" s="27">
         <v>21</v>
@@ -3010,7 +3063,7 @@
         <v>92</v>
       </c>
       <c r="J23" s="38" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="K23" s="40" t="s">
         <v>69</v>
@@ -3023,7 +3076,7 @@
         <v>74</v>
       </c>
       <c r="O23" s="8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="P23" s="63" t="s">
         <v>19</v>
@@ -3032,16 +3085,16 @@
         <v>6</v>
       </c>
       <c r="R23" s="11" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="S23" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="T23" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="U23" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="T23" s="11" t="s">
-        <v>193</v>
-      </c>
-      <c r="U23" s="1" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3055,14 +3108,14 @@
         <v>97</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E24" s="26" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F24" s="35"/>
       <c r="G24" s="37" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H24" s="27">
         <v>22</v>
@@ -3071,7 +3124,7 @@
         <v>92</v>
       </c>
       <c r="J24" s="38" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="K24" s="40" t="s">
         <v>69</v>
@@ -3084,7 +3137,7 @@
         <v>82</v>
       </c>
       <c r="O24" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="P24" s="63" t="s">
         <v>19</v>
@@ -3093,16 +3146,16 @@
         <v>6</v>
       </c>
       <c r="R24" s="25" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="S24" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="T24" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="U24" s="34" t="s">
         <v>174</v>
-      </c>
-      <c r="T24" s="25" t="s">
-        <v>194</v>
-      </c>
-      <c r="U24" s="34" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="25" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3116,14 +3169,14 @@
         <v>97</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E25" s="26" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F25" s="35"/>
       <c r="G25" s="37" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="H25" s="27">
         <v>23</v>
@@ -3132,7 +3185,7 @@
         <v>92</v>
       </c>
       <c r="J25" s="38" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="K25" s="40" t="s">
         <v>69</v>
@@ -3145,7 +3198,7 @@
         <v>54</v>
       </c>
       <c r="O25" s="47" t="s">
-        <v>116</v>
+        <v>239</v>
       </c>
       <c r="P25" s="63" t="s">
         <v>20</v>
@@ -3154,16 +3207,16 @@
         <v>6</v>
       </c>
       <c r="R25" s="25" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="S25" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="T25" s="25" t="s">
+        <v>235</v>
+      </c>
+      <c r="U25" s="34" t="s">
         <v>174</v>
-      </c>
-      <c r="T25" s="25" t="s">
-        <v>187</v>
-      </c>
-      <c r="U25" s="34" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3177,14 +3230,14 @@
         <v>97</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E26" s="26" t="s">
         <v>100</v>
       </c>
       <c r="F26" s="35"/>
       <c r="G26" s="37" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H26" s="27">
         <v>24</v>
@@ -3193,7 +3246,7 @@
         <v>92</v>
       </c>
       <c r="J26" s="38" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="K26" s="40" t="s">
         <v>69</v>
@@ -3206,7 +3259,7 @@
         <v>62</v>
       </c>
       <c r="O26" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="P26" s="63" t="s">
         <v>19</v>
@@ -3215,16 +3268,16 @@
         <v>6</v>
       </c>
       <c r="R26" s="25" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="S26" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="T26" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="U26" s="34" t="s">
         <v>174</v>
-      </c>
-      <c r="T26" s="25" t="s">
-        <v>179</v>
-      </c>
-      <c r="U26" s="34" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3238,14 +3291,14 @@
         <v>97</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E27" s="26" t="s">
         <v>100</v>
       </c>
       <c r="F27" s="35"/>
       <c r="G27" s="37" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="H27" s="27">
         <v>25</v>
@@ -3254,7 +3307,7 @@
         <v>92</v>
       </c>
       <c r="J27" s="38" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="K27" s="40" t="s">
         <v>70</v>
@@ -3271,19 +3324,19 @@
         <v>20</v>
       </c>
       <c r="Q27" s="59" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="R27" s="24" t="s">
+        <v>194</v>
+      </c>
+      <c r="S27" s="24" t="s">
+        <v>195</v>
+      </c>
+      <c r="T27" s="24" t="s">
+        <v>224</v>
+      </c>
+      <c r="U27" s="33" t="s">
         <v>197</v>
-      </c>
-      <c r="S27" s="24" t="s">
-        <v>198</v>
-      </c>
-      <c r="T27" s="24" t="s">
-        <v>227</v>
-      </c>
-      <c r="U27" s="33" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="28" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3297,12 +3350,12 @@
         <v>97</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E28" s="26"/>
       <c r="F28" s="35"/>
       <c r="G28" s="37" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="H28" s="27">
         <v>26</v>
@@ -3311,7 +3364,7 @@
         <v>91</v>
       </c>
       <c r="J28" s="38" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="K28" s="40" t="s">
         <v>69</v>
@@ -3324,7 +3377,7 @@
       </c>
       <c r="N28" s="9"/>
       <c r="O28" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="P28" s="63" t="s">
         <v>19</v>
@@ -3333,16 +3386,16 @@
         <v>6</v>
       </c>
       <c r="R28" s="25" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="S28" s="25" t="s">
+        <v>162</v>
+      </c>
+      <c r="T28" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="U28" s="34" t="s">
         <v>164</v>
-      </c>
-      <c r="T28" s="25" t="s">
-        <v>172</v>
-      </c>
-      <c r="U28" s="34" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="29" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3356,12 +3409,12 @@
         <v>97</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E29" s="26"/>
       <c r="F29" s="35"/>
       <c r="G29" s="37" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H29" s="27">
         <v>27</v>
@@ -3370,7 +3423,7 @@
         <v>92</v>
       </c>
       <c r="J29" s="38" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="K29" s="40" t="s">
         <v>69</v>
@@ -3383,7 +3436,7 @@
         <v>73</v>
       </c>
       <c r="O29" s="47" t="s">
-        <v>116</v>
+        <v>240</v>
       </c>
       <c r="P29" s="63" t="s">
         <v>19</v>
@@ -3392,16 +3445,16 @@
         <v>6</v>
       </c>
       <c r="R29" s="25" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="S29" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="T29" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="U29" s="34" t="s">
         <v>174</v>
-      </c>
-      <c r="T29" s="25" t="s">
-        <v>195</v>
-      </c>
-      <c r="U29" s="34" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="30" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3415,14 +3468,14 @@
         <v>97</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E30" s="26" t="s">
         <v>100</v>
       </c>
       <c r="F30" s="35"/>
       <c r="G30" s="37" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H30" s="27">
         <v>28</v>
@@ -3431,7 +3484,7 @@
         <v>92</v>
       </c>
       <c r="J30" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="K30" s="40" t="s">
         <v>69</v>
@@ -3444,7 +3497,7 @@
         <v>62</v>
       </c>
       <c r="O30" s="8" t="s">
-        <v>116</v>
+        <v>243</v>
       </c>
       <c r="P30" s="63" t="s">
         <v>19</v>
@@ -3453,16 +3506,16 @@
         <v>7</v>
       </c>
       <c r="R30" s="25" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="S30" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="T30" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="U30" s="34" t="s">
         <v>174</v>
-      </c>
-      <c r="T30" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="U30" s="34" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="31" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3481,7 +3534,7 @@
       <c r="E31" s="26"/>
       <c r="F31" s="35"/>
       <c r="G31" s="37" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H31" s="27">
         <v>29</v>
@@ -3490,7 +3543,7 @@
         <v>92</v>
       </c>
       <c r="J31" s="38" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="K31" s="40" t="s">
         <v>69</v>
@@ -3503,7 +3556,7 @@
         <v>64</v>
       </c>
       <c r="O31" s="47" t="s">
-        <v>116</v>
+        <v>244</v>
       </c>
       <c r="P31" s="63" t="s">
         <v>19</v>
@@ -3512,16 +3565,16 @@
         <v>10</v>
       </c>
       <c r="R31" s="25" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="S31" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="T31" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="U31" s="34" t="s">
         <v>174</v>
-      </c>
-      <c r="T31" s="25" t="s">
-        <v>182</v>
-      </c>
-      <c r="U31" s="34" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="32" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3540,7 +3593,7 @@
       <c r="E32" s="26"/>
       <c r="F32" s="35"/>
       <c r="G32" s="37" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H32" s="27">
         <v>30</v>
@@ -3549,7 +3602,7 @@
         <v>92</v>
       </c>
       <c r="J32" s="38" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="K32" s="40" t="s">
         <v>69</v>
@@ -3562,7 +3615,7 @@
         <v>64</v>
       </c>
       <c r="O32" s="47" t="s">
-        <v>116</v>
+        <v>245</v>
       </c>
       <c r="P32" s="63" t="s">
         <v>19</v>
@@ -3571,16 +3624,16 @@
         <v>11</v>
       </c>
       <c r="R32" s="25" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="S32" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="T32" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="U32" s="34" t="s">
         <v>174</v>
-      </c>
-      <c r="T32" s="25" t="s">
-        <v>183</v>
-      </c>
-      <c r="U32" s="34" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="33" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3599,7 +3652,7 @@
       <c r="E33" s="26"/>
       <c r="F33" s="35"/>
       <c r="G33" s="37" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H33" s="27">
         <v>31</v>
@@ -3608,7 +3661,7 @@
         <v>92</v>
       </c>
       <c r="J33" s="38" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K33" s="40" t="s">
         <v>69</v>
@@ -3621,7 +3674,7 @@
         <v>64</v>
       </c>
       <c r="O33" s="47" t="s">
-        <v>116</v>
+        <v>246</v>
       </c>
       <c r="P33" s="63" t="s">
         <v>19</v>
@@ -3630,16 +3683,16 @@
         <v>12</v>
       </c>
       <c r="R33" s="25" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="S33" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="T33" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="U33" s="34" t="s">
         <v>174</v>
-      </c>
-      <c r="T33" s="25" t="s">
-        <v>184</v>
-      </c>
-      <c r="U33" s="34" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="34" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3658,7 +3711,7 @@
       <c r="E34" s="26"/>
       <c r="F34" s="35"/>
       <c r="G34" s="37" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="H34" s="27">
         <v>32</v>
@@ -3667,7 +3720,7 @@
         <v>92</v>
       </c>
       <c r="J34" s="38" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="K34" s="40" t="s">
         <v>69</v>
@@ -3710,7 +3763,7 @@
         <v>92</v>
       </c>
       <c r="J35" s="38" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="K35" s="40" t="s">
         <v>69</v>
@@ -3723,7 +3776,7 @@
         <v>23</v>
       </c>
       <c r="O35" s="8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="P35" s="63" t="s">
         <v>19</v>
@@ -3732,16 +3785,16 @@
         <v>6</v>
       </c>
       <c r="R35" s="11" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="S35" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="T35" s="41" t="s">
+        <v>189</v>
+      </c>
+      <c r="U35" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="T35" s="41" t="s">
-        <v>191</v>
-      </c>
-      <c r="U35" s="1" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
@@ -3760,7 +3813,7 @@
       <c r="E36" s="26"/>
       <c r="F36" s="35"/>
       <c r="G36" s="37" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="H36" s="27">
         <v>34</v>
@@ -3769,7 +3822,7 @@
         <v>92</v>
       </c>
       <c r="J36" s="38" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="K36" s="40" t="s">
         <v>69</v>
@@ -3789,20 +3842,28 @@
         <v>6</v>
       </c>
       <c r="R36" s="11" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="S36" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="T36" s="41" t="s">
+        <v>219</v>
+      </c>
+      <c r="U36" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="T36" s="41" t="s">
-        <v>222</v>
-      </c>
-      <c r="U36" s="1" t="s">
-        <v>176</v>
-      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="O37" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="M1:N1"/>
@@ -3818,11 +3879,6 @@
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Solicitudes de video y escaletas ajustadas
Se eliminan las peticiones de nuevos audios y videos
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion01/ESCALETA_CN_09_01_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion01/ESCALETA_CN_09_01_CO.xlsx
@@ -332,9 +332,6 @@
     <t>Interactivo que muestra el proceso de síntesis de proteínas a partir del ADN</t>
   </si>
   <si>
-    <t xml:space="preserve">Se debe hacer una animación del proceso de síntesis de proteínas a partir del ADN, pasando por el ARN. Esta aniumación es muy resumida: no de explican términos como ligasa o polimerasa, no se habla de condones ni de tipor de ARN. Se muestra que del ADN se hace ARN en un proceso llamado transcripción, y que ese ARN es usado por los ribosomas para ensamblar proteínas en el proceso llamado traducción. Se puede usar como modelo una célula eucariótica. </t>
-  </si>
-  <si>
     <t>Los ácidos nucleicos</t>
   </si>
   <si>
@@ -452,9 +449,6 @@
     <t>Las preguntas deben incluir los temas transcripción, traducción, código genético y regulación</t>
   </si>
   <si>
-    <t>En la animación se explica la regulación genética, y en las preguntas se indaga sobre las consecuencias de las fallas de la regulación en distintos puntos en la transcripción y la traducción.</t>
-  </si>
-  <si>
     <t>Una falla molecular: el cáncer</t>
   </si>
   <si>
@@ -509,21 +503,9 @@
     <t>RF_01_01_CO</t>
   </si>
   <si>
-    <t>Recurso F12-02</t>
-  </si>
-  <si>
-    <t>Recurso F12-03</t>
-  </si>
-  <si>
-    <t>Recurso F12-04</t>
-  </si>
-  <si>
     <t>Recurso F13-01</t>
   </si>
   <si>
-    <t>Recurso F4-01</t>
-  </si>
-  <si>
     <t>Recurso F10-01</t>
   </si>
   <si>
@@ -575,9 +557,6 @@
     <t>Recurso M9B-01</t>
   </si>
   <si>
-    <t>Recurso M3B-01</t>
-  </si>
-  <si>
     <t>Recurso M15A-01</t>
   </si>
   <si>
@@ -590,9 +569,6 @@
     <t>Recurso M1C-01</t>
   </si>
   <si>
-    <t>Recurso M5B-01</t>
-  </si>
-  <si>
     <t>4º ESO</t>
   </si>
   <si>
@@ -651,9 +627,6 @@
   </si>
   <si>
     <t>La transcripción y la traducción</t>
-  </si>
-  <si>
-    <t>Explicar el código genético, aprovechando la pestaña de información en cada diapositiva. Primero se presenta el código, y luego se dan explicaciones y ejemplos usando codones específicos. Se debe también hablar de codones de inicio y parada. Al final, se pone una secuencia de varios codones (incluyendo inicio y parada) y se escribe la proteína que haría. Un buen ejemplo es la oxitocina, que tiene sólo 9 aminoácidos.</t>
   </si>
   <si>
     <t>Interactivo que explica qué es y como se usa el código genético</t>
@@ -696,9 +669,6 @@
 términos: Ribonucleótido, ribosa, A U C G, cadena sencilla. Proponer más términos, pero cuidando que no apliquen para ambos tipos de molécula. </t>
   </si>
   <si>
-    <t xml:space="preserve">Asociar 1 sonido 1 texto (M3B). Los audios contienen descripciones y los textos el término descrito. Por ejemplo: Audio “moléculas pequeñas compuestas principalmente por carbono, hidrógeno, oxígeno y nitrógeno” y el texto asociado es “Aminoácidos”. </t>
-  </si>
-  <si>
     <t>Cada pestaña es un tipo de molécula. Se presentan el ADN y el ARN (en dos pestañas aparte) aclarando que ambas moléculas son ácidos nucléicos y presentando los nucleótidos. Luego se presentan las proteínas, y se explica que se conforman de aminoácidos. Recordar explicar las moléculas de manera sencilla, sin olvidar que los estudiantes de este curso no han visto química orgánica.</t>
   </si>
   <si>
@@ -706,9 +676,6 @@
 </t>
   </si>
   <si>
-    <t>Se hace un video que muestre el proceso de replicación del ADN</t>
-  </si>
-  <si>
     <t>Se escribe el proceso de replicación del ADN es frases cortas, para que el estudiante ordene según la secuancia en la que se da cada paso descrito.</t>
   </si>
   <si>
@@ -718,12 +685,6 @@
     <t>Preguntas sobre replicación del ADN y mutaciones.</t>
   </si>
   <si>
-    <t>Se hace un video que muestre el proceso de transcripción del ADN</t>
-  </si>
-  <si>
-    <t>Se hace un video que muestre el proceso de traducción del ADN</t>
-  </si>
-  <si>
     <t>Los estudiantes ordenan la secuencia de eventos ocurridos durante la traducción.</t>
   </si>
   <si>
@@ -764,6 +725,45 @@
   </si>
   <si>
     <t>Refuerza tu aprendizaje: El cáncer</t>
+  </si>
+  <si>
+    <t>Se debe hacer una presentación del proceso de síntesis de proteínas a partir del ADN, pasando por el ARN. Esta presentación es muy resumida: no de explican términos como ligasa o polimerasa, no se habla de codones ni de tipos de ARN. Se muestra que a partir del ADN se hace ARN en un proceso llamado transcripción, y que ese ARN es usado por los ribosomas para ensamblar proteínas en el proceso llamado traducción. Se puede usar como modelo una célula eucariótica. En las preguntas se cuestiona sobre la importancia de un evento o molécula, por ejemplo la importancia de que el ADN permaneza en el núcleo, o se refuerza la comprensión de los detalles de lo que está pasando en cada momento (la molécula de ARN recien formada, ¿tiene doble cadena o cadena sencilla?).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asociar textos que contienen descripciones con palabras que son los términos descritos. Por ejemplo: texto “moléculas pequeñas compuestas principalmente por carbono, hidrógeno, oxígeno y nitrógeno” y la palabra asociada es “Aminoácidos”. </t>
+  </si>
+  <si>
+    <t>Recurso M1B-02</t>
+  </si>
+  <si>
+    <t>Recurso F13B-01</t>
+  </si>
+  <si>
+    <t>Se muestra paso a paso el proceso de replicación del ADN. Cada pestaña es un paso.</t>
+  </si>
+  <si>
+    <t>Se muestra paso a paso el proceso de transcrpción del ADN. Cada pestaña es un paso.</t>
+  </si>
+  <si>
+    <t>Se muestra paso a paso el proceso de traducción del ADN. Cada pestaña es un paso.</t>
+  </si>
+  <si>
+    <t>Recurso F13-02</t>
+  </si>
+  <si>
+    <t>Recurso F13-03</t>
+  </si>
+  <si>
+    <t>En la presentación se explica la regulación genética, y en las preguntas se indaga sobre las consecuencias de las fallas de la regulación en distintos puntos en la transcripción y la traducción.</t>
+  </si>
+  <si>
+    <t>Recurso F4-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explicar el código genético. Primero se presenta el código, y luego se dan explicaciones y ejemplos usando codones específicos. Se debe hablar de codones de inicio y parada. Desúés, se pone una secuencia de varios codones (incluyendo inicio y parada) y se escribe la proteína que haría. Un buen ejemplo es la oxitocina, que tiene sólo 9 aminoácidos. Para cumplir el requisito de tener más de una imagen en el menú principal, se puede tener uan rpesentación que explique qué es el código genético, en donde se dan todas las explicaciones pertinentes, y otra que se enfoque en cómo se usa, no ya explicando nada sino haciendo el ejercicio de determinar la proteína a partir de la secuencia de ARN. Es importante resaltar que el código genético funciona con ARN y no con ADN. Se puede hacer una tercera presentación en el menú que lleve el ejercicio más lejos: pasar de proteína a ARN, y luego de ARN  a ADN. A partir de la proteina se determian el gen (se ignoran cosas relativas a la edición de proteínas). </t>
+  </si>
+  <si>
+    <t>Recurso F6-01</t>
   </si>
 </sst>
 </file>
@@ -808,7 +808,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -869,6 +869,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="27">
     <border>
@@ -1030,19 +1036,6 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -1210,12 +1203,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1299,7 +1301,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1318,26 +1320,26 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1345,38 +1347,32 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1392,18 +1388,18 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1418,6 +1414,21 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1702,8 +1713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="K3" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1733,94 +1744,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="64" t="s">
+      <c r="B1" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="64" t="s">
+      <c r="C1" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="64" t="s">
+      <c r="D1" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="64" t="s">
+      <c r="E1" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="66" t="s">
+      <c r="F1" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="64" t="s">
+      <c r="G1" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="64" t="s">
+      <c r="H1" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="64" t="s">
+      <c r="I1" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="72" t="s">
+      <c r="J1" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="72" t="s">
+      <c r="K1" s="70" t="s">
         <v>71</v>
       </c>
-      <c r="L1" s="66" t="s">
+      <c r="L1" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="68" t="s">
+      <c r="M1" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="69"/>
-      <c r="O1" s="64" t="s">
+      <c r="N1" s="67"/>
+      <c r="O1" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="64" t="s">
+      <c r="P1" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="70" t="s">
+      <c r="Q1" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="64" t="s">
+      <c r="R1" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="64" t="s">
+      <c r="S1" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="64" t="s">
+      <c r="T1" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="64" t="s">
+      <c r="U1" s="62" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="5" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="65"/>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="73"/>
-      <c r="L2" s="67"/>
+      <c r="A2" s="63"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="65"/>
       <c r="M2" s="15" t="s">
         <v>87</v>
       </c>
       <c r="N2" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="O2" s="65"/>
-      <c r="P2" s="65"/>
-      <c r="Q2" s="71"/>
-      <c r="R2" s="65"/>
-      <c r="S2" s="65"/>
-      <c r="T2" s="65"/>
-      <c r="U2" s="65"/>
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
+      <c r="Q2" s="69"/>
+      <c r="R2" s="63"/>
+      <c r="S2" s="63"/>
+      <c r="T2" s="63"/>
+      <c r="U2" s="63"/>
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="28" t="s">
@@ -1836,11 +1847,11 @@
         <v>99</v>
       </c>
       <c r="E3" s="30"/>
-      <c r="F3" s="52" t="s">
-        <v>202</v>
-      </c>
-      <c r="G3" s="54" t="s">
-        <v>203</v>
+      <c r="F3" s="51" t="s">
+        <v>194</v>
+      </c>
+      <c r="G3" s="53" t="s">
+        <v>195</v>
       </c>
       <c r="H3" s="31">
         <v>1</v>
@@ -1855,32 +1866,32 @@
         <v>69</v>
       </c>
       <c r="L3" s="16" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="M3" s="17" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="N3" s="17"/>
       <c r="O3" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="P3" s="42" t="s">
+        <v>234</v>
+      </c>
+      <c r="P3" s="75" t="s">
         <v>19</v>
       </c>
       <c r="Q3" s="18">
         <v>6</v>
       </c>
       <c r="R3" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="S3" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="T3" s="19" t="s">
         <v>158</v>
       </c>
-      <c r="S3" s="19" t="s">
+      <c r="U3" s="20" t="s">
         <v>159</v>
-      </c>
-      <c r="T3" s="19" t="s">
-        <v>160</v>
-      </c>
-      <c r="U3" s="20" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1900,48 +1911,48 @@
         <v>100</v>
       </c>
       <c r="F4" s="35"/>
-      <c r="G4" s="56" t="s">
-        <v>241</v>
+      <c r="G4" s="55" t="s">
+        <v>228</v>
       </c>
       <c r="H4" s="27">
         <v>2</v>
       </c>
-      <c r="I4" s="44" t="s">
+      <c r="I4" s="43" t="s">
         <v>92</v>
       </c>
-      <c r="J4" s="45" t="s">
-        <v>204</v>
-      </c>
-      <c r="K4" s="46" t="s">
+      <c r="J4" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="K4" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="L4" s="47" t="s">
+      <c r="L4" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="M4" s="48"/>
-      <c r="N4" s="48" t="s">
+      <c r="M4" s="47"/>
+      <c r="N4" s="47" t="s">
         <v>62</v>
       </c>
-      <c r="O4" s="47" t="s">
-        <v>221</v>
-      </c>
-      <c r="P4" s="42" t="s">
+      <c r="O4" s="46" t="s">
+        <v>212</v>
+      </c>
+      <c r="P4" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="Q4" s="49">
+      <c r="Q4" s="48">
         <v>6</v>
       </c>
-      <c r="R4" s="50" t="s">
-        <v>168</v>
-      </c>
-      <c r="S4" s="50" t="s">
-        <v>169</v>
-      </c>
-      <c r="T4" s="50" t="s">
-        <v>172</v>
-      </c>
-      <c r="U4" s="51" t="s">
-        <v>171</v>
+      <c r="R4" s="49" t="s">
+        <v>162</v>
+      </c>
+      <c r="S4" s="49" t="s">
+        <v>163</v>
+      </c>
+      <c r="T4" s="49" t="s">
+        <v>166</v>
+      </c>
+      <c r="U4" s="50" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1954,11 +1965,11 @@
       <c r="C5" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="D5" s="55" t="s">
+      <c r="D5" s="54" t="s">
         <v>101</v>
       </c>
       <c r="E5" s="26"/>
-      <c r="F5" s="53"/>
+      <c r="F5" s="52"/>
       <c r="G5" s="37" t="s">
         <v>101</v>
       </c>
@@ -1969,7 +1980,7 @@
         <v>91</v>
       </c>
       <c r="J5" s="38" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K5" s="40" t="s">
         <v>69</v>
@@ -1978,29 +1989,29 @@
         <v>31</v>
       </c>
       <c r="M5" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="N5" s="9"/>
       <c r="O5" s="8" t="s">
-        <v>225</v>
-      </c>
-      <c r="P5" s="42" t="s">
+        <v>215</v>
+      </c>
+      <c r="P5" s="77" t="s">
         <v>19</v>
       </c>
       <c r="Q5" s="12">
         <v>6</v>
       </c>
       <c r="R5" s="11" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="S5" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="T5" s="41" t="s">
+        <v>237</v>
+      </c>
+      <c r="U5" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="T5" s="41" t="s">
-        <v>165</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2013,13 +2024,13 @@
       <c r="C6" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="D6" s="55" t="s">
+      <c r="D6" s="54" t="s">
         <v>101</v>
       </c>
       <c r="E6" s="26"/>
       <c r="F6" s="35"/>
       <c r="G6" s="37" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H6" s="27">
         <v>4</v>
@@ -2028,7 +2039,7 @@
         <v>92</v>
       </c>
       <c r="J6" s="38" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K6" s="40" t="s">
         <v>69</v>
@@ -2040,26 +2051,26 @@
       <c r="N6" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="O6" s="47" t="s">
-        <v>222</v>
-      </c>
-      <c r="P6" s="62" t="s">
+      <c r="O6" s="46" t="s">
+        <v>213</v>
+      </c>
+      <c r="P6" s="76" t="s">
         <v>19</v>
       </c>
       <c r="Q6" s="12">
         <v>6</v>
       </c>
       <c r="R6" s="11" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="S6" s="11" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="T6" s="41" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2072,17 +2083,17 @@
       <c r="C7" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="D7" s="55" t="s">
+      <c r="D7" s="54" t="s">
         <v>101</v>
       </c>
       <c r="E7" s="26" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F7" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="G7" s="37" t="s">
         <v>108</v>
-      </c>
-      <c r="G7" s="37" t="s">
-        <v>109</v>
       </c>
       <c r="H7" s="27">
         <v>5</v>
@@ -2091,7 +2102,7 @@
         <v>91</v>
       </c>
       <c r="J7" s="38" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="K7" s="40" t="s">
         <v>70</v>
@@ -2101,24 +2112,24 @@
       </c>
       <c r="M7" s="9"/>
       <c r="N7" s="9"/>
-      <c r="O7" s="47"/>
-      <c r="P7" s="63" t="s">
+      <c r="O7" s="46"/>
+      <c r="P7" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="Q7" s="59" t="s">
-        <v>190</v>
+      <c r="Q7" s="58" t="s">
+        <v>182</v>
       </c>
       <c r="R7" s="24" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="S7" s="24" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="T7" s="24" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="U7" s="33" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2131,17 +2142,17 @@
       <c r="C8" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="D8" s="55" t="s">
+      <c r="D8" s="54" t="s">
         <v>101</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F8" s="35" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G8" s="37" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H8" s="27">
         <v>6</v>
@@ -2150,7 +2161,7 @@
         <v>92</v>
       </c>
       <c r="J8" s="38" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K8" s="40" t="s">
         <v>69</v>
@@ -2158,30 +2169,30 @@
       <c r="L8" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="M8" s="9"/>
+      <c r="M8" s="79"/>
       <c r="N8" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="O8" s="47" t="s">
-        <v>226</v>
-      </c>
-      <c r="P8" s="63" t="s">
+      <c r="O8" s="46" t="s">
+        <v>216</v>
+      </c>
+      <c r="P8" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="Q8" s="59">
+      <c r="Q8" s="58">
         <v>6</v>
       </c>
       <c r="R8" s="24" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="S8" s="24" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="T8" s="24" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="U8" s="33" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2194,17 +2205,17 @@
       <c r="C9" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="D9" s="55" t="s">
+      <c r="D9" s="54" t="s">
         <v>101</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F9" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="G9" s="56" t="s">
         <v>112</v>
-      </c>
-      <c r="G9" s="57" t="s">
-        <v>113</v>
       </c>
       <c r="H9" s="27">
         <v>7</v>
@@ -2213,7 +2224,7 @@
         <v>92</v>
       </c>
       <c r="J9" s="38" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K9" s="40" t="s">
         <v>69</v>
@@ -2221,30 +2232,30 @@
       <c r="L9" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="M9" s="9"/>
+      <c r="M9" s="79"/>
       <c r="N9" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="O9" s="47" t="s">
-        <v>223</v>
-      </c>
-      <c r="P9" s="63" t="s">
+      <c r="O9" s="46" t="s">
+        <v>214</v>
+      </c>
+      <c r="P9" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="Q9" s="59">
+      <c r="Q9" s="58">
         <v>6</v>
       </c>
       <c r="R9" s="24" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="S9" s="24" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="T9" s="24" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="U9" s="33" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2257,17 +2268,17 @@
       <c r="C10" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="D10" s="55" t="s">
+      <c r="D10" s="54" t="s">
         <v>101</v>
       </c>
       <c r="E10" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="F10" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="F10" s="35" t="s">
+      <c r="G10" s="55" t="s">
         <v>116</v>
-      </c>
-      <c r="G10" s="56" t="s">
-        <v>117</v>
       </c>
       <c r="H10" s="27">
         <v>8</v>
@@ -2276,7 +2287,7 @@
         <v>92</v>
       </c>
       <c r="J10" s="38" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="K10" s="40" t="s">
         <v>69</v>
@@ -2284,30 +2295,30 @@
       <c r="L10" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="M10" s="9"/>
+      <c r="M10" s="79"/>
       <c r="N10" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="O10" s="47" t="s">
-        <v>224</v>
-      </c>
-      <c r="P10" s="63" t="s">
+        <v>73</v>
+      </c>
+      <c r="O10" s="46" t="s">
+        <v>235</v>
+      </c>
+      <c r="P10" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="Q10" s="60">
+      <c r="Q10" s="59">
         <v>6</v>
       </c>
       <c r="R10" s="11" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="S10" s="11" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="T10" s="41" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2324,13 +2335,13 @@
         <v>101</v>
       </c>
       <c r="E11" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="F11" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="F11" s="35" t="s">
-        <v>116</v>
-      </c>
-      <c r="G11" s="58" t="s">
-        <v>197</v>
+      <c r="G11" s="57" t="s">
+        <v>189</v>
       </c>
       <c r="H11" s="27">
         <v>9</v>
@@ -2339,7 +2350,7 @@
         <v>92</v>
       </c>
       <c r="J11" s="38" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="K11" s="40" t="s">
         <v>69</v>
@@ -2347,30 +2358,30 @@
       <c r="L11" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="M11" s="9"/>
+      <c r="M11" s="79"/>
       <c r="N11" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="O11" s="47" t="s">
-        <v>236</v>
-      </c>
-      <c r="P11" s="63" t="s">
+      <c r="O11" s="46" t="s">
+        <v>223</v>
+      </c>
+      <c r="P11" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="Q11" s="59">
+      <c r="Q11" s="58">
         <v>6</v>
       </c>
       <c r="R11" s="24" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="S11" s="24" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="T11" s="24" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="U11" s="33" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2383,7 +2394,7 @@
       <c r="C12" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="D12" s="55" t="s">
+      <c r="D12" s="54" t="s">
         <v>101</v>
       </c>
       <c r="E12" s="26" t="s">
@@ -2391,7 +2402,7 @@
       </c>
       <c r="F12" s="35"/>
       <c r="G12" s="37" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="H12" s="27">
         <v>10</v>
@@ -2400,7 +2411,7 @@
         <v>92</v>
       </c>
       <c r="J12" s="38" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="K12" s="40" t="s">
         <v>69</v>
@@ -2408,30 +2419,30 @@
       <c r="L12" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="M12" s="9"/>
+      <c r="M12" s="79"/>
       <c r="N12" s="9" t="s">
         <v>62</v>
       </c>
       <c r="O12" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="P12" s="63" t="s">
+        <v>117</v>
+      </c>
+      <c r="P12" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="Q12" s="59">
+      <c r="Q12" s="58">
         <v>6</v>
       </c>
       <c r="R12" s="24" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="S12" s="24" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="T12" s="24" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="U12" s="33" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2445,14 +2456,14 @@
         <v>97</v>
       </c>
       <c r="D13" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="E13" s="26" t="s">
         <v>119</v>
-      </c>
-      <c r="E13" s="26" t="s">
-        <v>120</v>
       </c>
       <c r="F13" s="35"/>
       <c r="G13" s="37" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="H13" s="27">
         <v>11</v>
@@ -2461,7 +2472,7 @@
         <v>91</v>
       </c>
       <c r="J13" s="38" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K13" s="40" t="s">
         <v>69</v>
@@ -2469,30 +2480,30 @@
       <c r="L13" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="M13" s="9" t="s">
-        <v>44</v>
+      <c r="M13" s="79" t="s">
+        <v>45</v>
       </c>
       <c r="N13" s="9"/>
-      <c r="O13" s="47" t="s">
-        <v>227</v>
-      </c>
-      <c r="P13" s="63" t="s">
+      <c r="O13" s="46" t="s">
+        <v>238</v>
+      </c>
+      <c r="P13" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="Q13" s="61">
+      <c r="Q13" s="60">
         <v>6</v>
       </c>
       <c r="R13" s="25" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="S13" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="T13" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="U13" s="34" t="s">
         <v>159</v>
-      </c>
-      <c r="T13" s="25" t="s">
-        <v>162</v>
-      </c>
-      <c r="U13" s="34" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2506,14 +2517,14 @@
         <v>97</v>
       </c>
       <c r="D14" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="E14" s="26" t="s">
         <v>119</v>
-      </c>
-      <c r="E14" s="26" t="s">
-        <v>120</v>
       </c>
       <c r="F14" s="35"/>
       <c r="G14" s="37" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H14" s="27">
         <v>12</v>
@@ -2522,7 +2533,7 @@
         <v>92</v>
       </c>
       <c r="J14" s="38" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K14" s="40" t="s">
         <v>69</v>
@@ -2530,30 +2541,30 @@
       <c r="L14" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="M14" s="9"/>
+      <c r="M14" s="79"/>
       <c r="N14" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="O14" s="47" t="s">
-        <v>228</v>
-      </c>
-      <c r="P14" s="63" t="s">
+      <c r="O14" s="46" t="s">
+        <v>217</v>
+      </c>
+      <c r="P14" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="Q14" s="61">
+      <c r="Q14" s="60">
         <v>6</v>
       </c>
       <c r="R14" s="25" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="S14" s="25" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="T14" s="25" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="U14" s="34" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2567,14 +2578,14 @@
         <v>97</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E15" s="26" t="s">
         <v>96</v>
       </c>
       <c r="F15" s="35"/>
       <c r="G15" s="37" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H15" s="27">
         <v>13</v>
@@ -2583,7 +2594,7 @@
         <v>91</v>
       </c>
       <c r="J15" s="38" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="K15" s="40" t="s">
         <v>70</v>
@@ -2591,26 +2602,26 @@
       <c r="L15" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="M15" s="9"/>
+      <c r="M15" s="79"/>
       <c r="N15" s="9"/>
       <c r="O15" s="8"/>
-      <c r="P15" s="63" t="s">
+      <c r="P15" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="Q15" s="61" t="s">
-        <v>190</v>
+      <c r="Q15" s="60" t="s">
+        <v>182</v>
       </c>
       <c r="R15" s="25" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="S15" s="25" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="T15" s="25" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="U15" s="34" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2624,14 +2635,14 @@
         <v>97</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E16" s="26" t="s">
         <v>96</v>
       </c>
       <c r="F16" s="35"/>
       <c r="G16" s="37" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="H16" s="27">
         <v>14</v>
@@ -2640,7 +2651,7 @@
         <v>92</v>
       </c>
       <c r="J16" s="38" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K16" s="40" t="s">
         <v>70</v>
@@ -2648,26 +2659,26 @@
       <c r="L16" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="M16" s="9"/>
+      <c r="M16" s="79"/>
       <c r="N16" s="9"/>
       <c r="O16" s="8"/>
-      <c r="P16" s="63" t="s">
+      <c r="P16" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="Q16" s="60" t="s">
-        <v>190</v>
+      <c r="Q16" s="59" t="s">
+        <v>182</v>
       </c>
       <c r="R16" s="11" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="S16" s="11" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="T16" s="11" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="U16" s="1" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2681,14 +2692,14 @@
         <v>97</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E17" s="26" t="s">
         <v>100</v>
       </c>
       <c r="F17" s="35"/>
       <c r="G17" s="37" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
       <c r="H17" s="27">
         <v>15</v>
@@ -2697,7 +2708,7 @@
         <v>92</v>
       </c>
       <c r="J17" s="38" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K17" s="40" t="s">
         <v>69</v>
@@ -2705,30 +2716,30 @@
       <c r="L17" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="M17" s="9"/>
+      <c r="M17" s="79"/>
       <c r="N17" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="O17" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="P17" s="63" t="s">
+      <c r="O17" s="46" t="s">
+        <v>219</v>
+      </c>
+      <c r="P17" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="Q17" s="60">
+      <c r="Q17" s="59">
         <v>6</v>
       </c>
       <c r="R17" s="11" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="S17" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="T17" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="T17" s="11" t="s">
-        <v>175</v>
-      </c>
       <c r="U17" s="1" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2742,14 +2753,14 @@
         <v>97</v>
       </c>
       <c r="D18" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="E18" s="26" t="s">
         <v>127</v>
-      </c>
-      <c r="E18" s="26" t="s">
-        <v>128</v>
       </c>
       <c r="F18" s="35"/>
       <c r="G18" s="37" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H18" s="27">
         <v>16</v>
@@ -2758,7 +2769,7 @@
         <v>91</v>
       </c>
       <c r="J18" s="38" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K18" s="40" t="s">
         <v>69</v>
@@ -2766,30 +2777,30 @@
       <c r="L18" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="M18" s="9" t="s">
-        <v>44</v>
+      <c r="M18" s="79" t="s">
+        <v>45</v>
       </c>
       <c r="N18" s="9"/>
-      <c r="O18" s="47" t="s">
-        <v>231</v>
-      </c>
-      <c r="P18" s="63" t="s">
+      <c r="O18" s="46" t="s">
+        <v>239</v>
+      </c>
+      <c r="P18" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="Q18" s="60">
+      <c r="Q18" s="59">
         <v>6</v>
       </c>
       <c r="R18" s="11" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="S18" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="T18" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="U18" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="T18" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="U18" s="1" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2803,14 +2814,14 @@
         <v>97</v>
       </c>
       <c r="D19" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="E19" s="26" t="s">
         <v>127</v>
-      </c>
-      <c r="E19" s="26" t="s">
-        <v>128</v>
       </c>
       <c r="F19" s="35"/>
       <c r="G19" s="37" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H19" s="27">
         <v>17</v>
@@ -2819,7 +2830,7 @@
         <v>92</v>
       </c>
       <c r="J19" s="38" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K19" s="40" t="s">
         <v>69</v>
@@ -2827,30 +2838,30 @@
       <c r="L19" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="M19" s="9"/>
+      <c r="M19" s="79"/>
       <c r="N19" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="O19" s="47" t="s">
-        <v>235</v>
-      </c>
-      <c r="P19" s="63" t="s">
+      <c r="O19" s="46" t="s">
+        <v>222</v>
+      </c>
+      <c r="P19" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="Q19" s="60">
+      <c r="Q19" s="59">
         <v>6</v>
       </c>
       <c r="R19" s="11" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="S19" s="11" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="T19" s="11" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="U19" s="1" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2864,14 +2875,14 @@
         <v>97</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E20" s="26" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F20" s="35"/>
       <c r="G20" s="37" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H20" s="27">
         <v>18</v>
@@ -2880,7 +2891,7 @@
         <v>91</v>
       </c>
       <c r="J20" s="38" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K20" s="40" t="s">
         <v>69</v>
@@ -2888,30 +2899,30 @@
       <c r="L20" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="M20" s="9" t="s">
-        <v>44</v>
+      <c r="M20" s="79" t="s">
+        <v>45</v>
       </c>
       <c r="N20" s="9"/>
-      <c r="O20" s="47" t="s">
-        <v>232</v>
-      </c>
-      <c r="P20" s="63" t="s">
+      <c r="O20" s="46" t="s">
+        <v>240</v>
+      </c>
+      <c r="P20" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="Q20" s="60">
+      <c r="Q20" s="59">
         <v>6</v>
       </c>
       <c r="R20" s="11" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="S20" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="T20" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="U20" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="T20" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="U20" s="1" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2925,14 +2936,14 @@
         <v>97</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E21" s="26" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F21" s="35"/>
       <c r="G21" s="37" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="H21" s="27">
         <v>19</v>
@@ -2941,7 +2952,7 @@
         <v>92</v>
       </c>
       <c r="J21" s="38" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K21" s="40" t="s">
         <v>70</v>
@@ -2949,26 +2960,26 @@
       <c r="L21" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="M21" s="9"/>
+      <c r="M21" s="79"/>
       <c r="N21" s="9"/>
       <c r="O21" s="8"/>
-      <c r="P21" s="63" t="s">
+      <c r="P21" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="Q21" s="61" t="s">
-        <v>190</v>
+      <c r="Q21" s="60" t="s">
+        <v>182</v>
       </c>
       <c r="R21" s="25" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="S21" s="25" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="T21" s="25" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="U21" s="34" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2982,16 +2993,16 @@
         <v>97</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E22" s="26" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F22" s="35" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G22" s="37" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H22" s="27">
         <v>20</v>
@@ -3000,7 +3011,7 @@
         <v>91</v>
       </c>
       <c r="J22" s="38" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="K22" s="40" t="s">
         <v>69</v>
@@ -3008,30 +3019,30 @@
       <c r="L22" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="M22" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="N22" s="9"/>
+      <c r="M22" s="79" t="s">
+        <v>36</v>
+      </c>
+      <c r="N22" s="79"/>
       <c r="O22" s="8" t="s">
-        <v>210</v>
-      </c>
-      <c r="P22" s="63" t="s">
+        <v>245</v>
+      </c>
+      <c r="P22" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="Q22" s="61">
+      <c r="Q22" s="60">
         <v>6</v>
       </c>
       <c r="R22" s="25" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="S22" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="T22" s="25" t="s">
+        <v>246</v>
+      </c>
+      <c r="U22" s="34" t="s">
         <v>159</v>
-      </c>
-      <c r="T22" s="25" t="s">
-        <v>166</v>
-      </c>
-      <c r="U22" s="34" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="23" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3045,16 +3056,16 @@
         <v>97</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E23" s="26" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F23" s="35" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G23" s="37" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H23" s="27">
         <v>21</v>
@@ -3063,7 +3074,7 @@
         <v>92</v>
       </c>
       <c r="J23" s="38" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K23" s="40" t="s">
         <v>69</v>
@@ -3071,30 +3082,30 @@
       <c r="L23" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="M23" s="9"/>
-      <c r="N23" s="9" t="s">
+      <c r="M23" s="79"/>
+      <c r="N23" s="79" t="s">
         <v>74</v>
       </c>
       <c r="O23" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="P23" s="63" t="s">
+        <v>140</v>
+      </c>
+      <c r="P23" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="Q23" s="60">
+      <c r="Q23" s="59">
         <v>6</v>
       </c>
       <c r="R23" s="11" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="S23" s="11" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="T23" s="11" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="U23" s="1" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3108,14 +3119,14 @@
         <v>97</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E24" s="26" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F24" s="35"/>
       <c r="G24" s="37" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H24" s="27">
         <v>22</v>
@@ -3124,38 +3135,38 @@
         <v>92</v>
       </c>
       <c r="J24" s="38" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K24" s="40" t="s">
         <v>69</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="M24" s="9"/>
-      <c r="N24" s="9" t="s">
-        <v>82</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="M24" s="79" t="s">
+        <v>35</v>
+      </c>
+      <c r="N24" s="79"/>
       <c r="O24" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="P24" s="63" t="s">
+        <v>243</v>
+      </c>
+      <c r="P24" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="Q24" s="61">
+      <c r="Q24" s="60">
         <v>6</v>
       </c>
       <c r="R24" s="25" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="S24" s="25" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="T24" s="25" t="s">
-        <v>189</v>
+        <v>244</v>
       </c>
       <c r="U24" s="34" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
     </row>
     <row r="25" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3169,14 +3180,14 @@
         <v>97</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E25" s="26" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F25" s="35"/>
       <c r="G25" s="37" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="H25" s="27">
         <v>23</v>
@@ -3185,7 +3196,7 @@
         <v>92</v>
       </c>
       <c r="J25" s="38" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="K25" s="40" t="s">
         <v>69</v>
@@ -3194,29 +3205,29 @@
         <v>32</v>
       </c>
       <c r="M25" s="9"/>
-      <c r="N25" s="9" t="s">
+      <c r="N25" s="79" t="s">
         <v>54</v>
       </c>
-      <c r="O25" s="47" t="s">
-        <v>233</v>
-      </c>
-      <c r="P25" s="63" t="s">
+      <c r="O25" s="46" t="s">
+        <v>220</v>
+      </c>
+      <c r="P25" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="Q25" s="61">
+      <c r="Q25" s="60">
         <v>6</v>
       </c>
       <c r="R25" s="25" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="S25" s="25" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="T25" s="25" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="U25" s="34" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3230,14 +3241,14 @@
         <v>97</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E26" s="26" t="s">
         <v>100</v>
       </c>
       <c r="F26" s="35"/>
       <c r="G26" s="37" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
       <c r="H26" s="27">
         <v>24</v>
@@ -3246,7 +3257,7 @@
         <v>92</v>
       </c>
       <c r="J26" s="38" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K26" s="40" t="s">
         <v>69</v>
@@ -3255,29 +3266,29 @@
         <v>32</v>
       </c>
       <c r="M26" s="9"/>
-      <c r="N26" s="9" t="s">
+      <c r="N26" s="79" t="s">
         <v>62</v>
       </c>
       <c r="O26" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="P26" s="63" t="s">
+        <v>141</v>
+      </c>
+      <c r="P26" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="Q26" s="61">
+      <c r="Q26" s="60">
         <v>6</v>
       </c>
       <c r="R26" s="25" t="s">
+        <v>162</v>
+      </c>
+      <c r="S26" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="T26" s="25" t="s">
         <v>168</v>
       </c>
-      <c r="S26" s="25" t="s">
-        <v>169</v>
-      </c>
-      <c r="T26" s="25" t="s">
-        <v>174</v>
-      </c>
       <c r="U26" s="34" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3291,14 +3302,14 @@
         <v>97</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E27" s="26" t="s">
         <v>100</v>
       </c>
       <c r="F27" s="35"/>
       <c r="G27" s="37" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
       <c r="H27" s="27">
         <v>25</v>
@@ -3307,7 +3318,7 @@
         <v>92</v>
       </c>
       <c r="J27" s="38" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="K27" s="40" t="s">
         <v>70</v>
@@ -3316,27 +3327,27 @@
         <v>32</v>
       </c>
       <c r="M27" s="9"/>
-      <c r="N27" s="9" t="s">
+      <c r="N27" s="79" t="s">
         <v>62</v>
       </c>
       <c r="O27" s="8"/>
-      <c r="P27" s="63" t="s">
+      <c r="P27" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="Q27" s="59" t="s">
-        <v>190</v>
+      <c r="Q27" s="58" t="s">
+        <v>182</v>
       </c>
       <c r="R27" s="24" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="S27" s="24" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="T27" s="24" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="U27" s="33" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
     </row>
     <row r="28" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3350,12 +3361,12 @@
         <v>97</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E28" s="26"/>
       <c r="F28" s="35"/>
       <c r="G28" s="37" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H28" s="27">
         <v>26</v>
@@ -3364,7 +3375,7 @@
         <v>91</v>
       </c>
       <c r="J28" s="38" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="K28" s="40" t="s">
         <v>69</v>
@@ -3377,25 +3388,25 @@
       </c>
       <c r="N28" s="9"/>
       <c r="O28" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="P28" s="63" t="s">
+        <v>146</v>
+      </c>
+      <c r="P28" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="Q28" s="61">
+      <c r="Q28" s="60">
         <v>6</v>
       </c>
       <c r="R28" s="25" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="S28" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="T28" s="25" t="s">
+        <v>161</v>
+      </c>
+      <c r="U28" s="34" t="s">
         <v>159</v>
-      </c>
-      <c r="T28" s="25" t="s">
-        <v>167</v>
-      </c>
-      <c r="U28" s="34" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="29" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3409,12 +3420,12 @@
         <v>97</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E29" s="26"/>
       <c r="F29" s="35"/>
       <c r="G29" s="37" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H29" s="27">
         <v>27</v>
@@ -3423,7 +3434,7 @@
         <v>92</v>
       </c>
       <c r="J29" s="38" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="K29" s="40" t="s">
         <v>69</v>
@@ -3435,26 +3446,26 @@
       <c r="N29" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="O29" s="47" t="s">
-        <v>234</v>
-      </c>
-      <c r="P29" s="63" t="s">
+      <c r="O29" s="46" t="s">
+        <v>221</v>
+      </c>
+      <c r="P29" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="Q29" s="61">
+      <c r="Q29" s="60">
         <v>6</v>
       </c>
       <c r="R29" s="25" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="S29" s="25" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="T29" s="25" t="s">
-        <v>181</v>
+        <v>236</v>
       </c>
       <c r="U29" s="34" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="30" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3468,14 +3479,14 @@
         <v>97</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E30" s="26" t="s">
         <v>100</v>
       </c>
       <c r="F30" s="35"/>
       <c r="G30" s="37" t="s">
-        <v>246</v>
+        <v>233</v>
       </c>
       <c r="H30" s="27">
         <v>28</v>
@@ -3484,7 +3495,7 @@
         <v>92</v>
       </c>
       <c r="J30" s="38" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="K30" s="40" t="s">
         <v>69</v>
@@ -3497,25 +3508,25 @@
         <v>62</v>
       </c>
       <c r="O30" s="8" t="s">
-        <v>237</v>
-      </c>
-      <c r="P30" s="63" t="s">
+        <v>224</v>
+      </c>
+      <c r="P30" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="Q30" s="61">
+      <c r="Q30" s="60">
         <v>7</v>
       </c>
       <c r="R30" s="25" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="S30" s="25" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="T30" s="25" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="U30" s="34" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="31" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3534,7 +3545,7 @@
       <c r="E31" s="26"/>
       <c r="F31" s="35"/>
       <c r="G31" s="37" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H31" s="27">
         <v>29</v>
@@ -3543,7 +3554,7 @@
         <v>92</v>
       </c>
       <c r="J31" s="38" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="K31" s="40" t="s">
         <v>69</v>
@@ -3555,26 +3566,26 @@
       <c r="N31" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="O31" s="47" t="s">
-        <v>238</v>
-      </c>
-      <c r="P31" s="63" t="s">
+      <c r="O31" s="46" t="s">
+        <v>225</v>
+      </c>
+      <c r="P31" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="Q31" s="61">
+      <c r="Q31" s="60">
         <v>10</v>
       </c>
       <c r="R31" s="25" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="S31" s="25" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="T31" s="25" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="U31" s="34" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="32" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3593,7 +3604,7 @@
       <c r="E32" s="26"/>
       <c r="F32" s="35"/>
       <c r="G32" s="37" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H32" s="27">
         <v>30</v>
@@ -3602,7 +3613,7 @@
         <v>92</v>
       </c>
       <c r="J32" s="38" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="K32" s="40" t="s">
         <v>69</v>
@@ -3614,26 +3625,26 @@
       <c r="N32" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="O32" s="47" t="s">
-        <v>239</v>
-      </c>
-      <c r="P32" s="63" t="s">
+      <c r="O32" s="46" t="s">
+        <v>226</v>
+      </c>
+      <c r="P32" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="Q32" s="61">
+      <c r="Q32" s="60">
         <v>11</v>
       </c>
       <c r="R32" s="25" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="S32" s="25" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="T32" s="25" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="U32" s="34" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="33" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3652,7 +3663,7 @@
       <c r="E33" s="26"/>
       <c r="F33" s="35"/>
       <c r="G33" s="37" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H33" s="27">
         <v>31</v>
@@ -3661,7 +3672,7 @@
         <v>92</v>
       </c>
       <c r="J33" s="38" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="K33" s="40" t="s">
         <v>69</v>
@@ -3673,26 +3684,26 @@
       <c r="N33" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="O33" s="47" t="s">
-        <v>240</v>
-      </c>
-      <c r="P33" s="63" t="s">
+      <c r="O33" s="46" t="s">
+        <v>227</v>
+      </c>
+      <c r="P33" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="Q33" s="61">
+      <c r="Q33" s="60">
         <v>12</v>
       </c>
       <c r="R33" s="25" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="S33" s="25" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="T33" s="25" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="U33" s="34" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="34" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3711,7 +3722,7 @@
       <c r="E34" s="26"/>
       <c r="F34" s="35"/>
       <c r="G34" s="37" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="H34" s="27">
         <v>32</v>
@@ -3720,7 +3731,7 @@
         <v>92</v>
       </c>
       <c r="J34" s="38" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="K34" s="40" t="s">
         <v>69</v>
@@ -3729,10 +3740,10 @@
       <c r="M34" s="9"/>
       <c r="N34" s="9"/>
       <c r="O34" s="8"/>
-      <c r="P34" s="63" t="s">
+      <c r="P34" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="Q34" s="60"/>
+      <c r="Q34" s="59"/>
       <c r="R34" s="11"/>
       <c r="S34" s="11"/>
       <c r="T34" s="41"/>
@@ -3763,7 +3774,7 @@
         <v>92</v>
       </c>
       <c r="J35" s="38" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="K35" s="40" t="s">
         <v>69</v>
@@ -3776,25 +3787,25 @@
         <v>23</v>
       </c>
       <c r="O35" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="P35" s="63" t="s">
+        <v>155</v>
+      </c>
+      <c r="P35" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="Q35" s="60">
+      <c r="Q35" s="59">
         <v>6</v>
       </c>
       <c r="R35" s="11" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="S35" s="11" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="T35" s="41" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="U35" s="1" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
@@ -3813,7 +3824,7 @@
       <c r="E36" s="26"/>
       <c r="F36" s="35"/>
       <c r="G36" s="37" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="H36" s="27">
         <v>34</v>
@@ -3822,7 +3833,7 @@
         <v>92</v>
       </c>
       <c r="J36" s="38" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="K36" s="40" t="s">
         <v>69</v>
@@ -3835,23 +3846,23 @@
         <v>63</v>
       </c>
       <c r="O36" s="8"/>
-      <c r="P36" s="63" t="s">
+      <c r="P36" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="Q36" s="60">
+      <c r="Q36" s="59">
         <v>6</v>
       </c>
       <c r="R36" s="11" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="S36" s="11" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="T36" s="41" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="U36" s="1" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
@@ -4593,40 +4604,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="64" t="s">
+      <c r="B1" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="64" t="s">
+      <c r="C1" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="64" t="s">
+      <c r="D1" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="64" t="s">
+      <c r="E1" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="64" t="s">
+      <c r="F1" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="74" t="s">
+      <c r="G1" s="72" t="s">
         <v>90</v>
       </c>
-      <c r="H1" s="64" t="s">
+      <c r="H1" s="62" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="65"/>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="76"/>
+      <c r="A2" s="63"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="74"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
@@ -4756,7 +4767,7 @@
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
       <c r="E13" s="13"/>
-      <c r="F13" s="43"/>
+      <c r="F13" s="42"/>
       <c r="G13" s="14"/>
       <c r="H13" s="9"/>
     </row>
@@ -4768,7 +4779,7 @@
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
       <c r="E14" s="13"/>
-      <c r="F14" s="43"/>
+      <c r="F14" s="42"/>
       <c r="G14" s="14"/>
       <c r="H14" s="9"/>
     </row>
@@ -4780,7 +4791,7 @@
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
       <c r="E15" s="13"/>
-      <c r="F15" s="43"/>
+      <c r="F15" s="42"/>
       <c r="G15" s="14"/>
       <c r="H15" s="9"/>
     </row>
@@ -4792,7 +4803,7 @@
       <c r="C16" s="13"/>
       <c r="D16" s="13"/>
       <c r="E16" s="13"/>
-      <c r="F16" s="43"/>
+      <c r="F16" s="42"/>
       <c r="G16" s="14"/>
       <c r="H16" s="9"/>
     </row>

</xml_diff>

<commit_message>
Cambios en descripción y nombre de los proyectos
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion01/ESCALETA_CN_09_01_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion01/ESCALETA_CN_09_01_CO.xlsx
@@ -464,13 +464,7 @@
     <t>Competencias: mutaciones y traducción</t>
   </si>
   <si>
-    <t>Competencias: el cáncer</t>
-  </si>
-  <si>
     <t>Actividad que propone identificar mutaciones en el ADN y su afectación en las proteínas</t>
-  </si>
-  <si>
-    <t>Actividad que propone organizar una exposición relacionada con diferentes tipos de cáncer</t>
   </si>
   <si>
     <t>Competencias: el rompecabezas de ADN</t>
@@ -773,6 +767,12 @@
   </si>
   <si>
     <t>Recurso F13-04</t>
+  </si>
+  <si>
+    <t>Proyecto: investigación acerca del cáncer</t>
+  </si>
+  <si>
+    <t>Actividad que guía el trabajo colaborativo sobre la investigación de diferentes tipos de cáncer</t>
   </si>
 </sst>
 </file>
@@ -1712,7 +1712,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1722,8 +1722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="F3" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1857,10 +1857,10 @@
       </c>
       <c r="E3" s="30"/>
       <c r="F3" s="51" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G3" s="53" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="H3" s="31">
         <v>1</v>
@@ -1882,7 +1882,7 @@
       </c>
       <c r="N3" s="17"/>
       <c r="O3" s="16" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="P3" s="62" t="s">
         <v>19</v>
@@ -1891,16 +1891,16 @@
         <v>6</v>
       </c>
       <c r="R3" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="S3" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="T3" s="19" t="s">
         <v>155</v>
       </c>
-      <c r="S3" s="19" t="s">
+      <c r="U3" s="20" t="s">
         <v>156</v>
-      </c>
-      <c r="T3" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="U3" s="20" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1921,7 +1921,7 @@
       </c>
       <c r="F4" s="35"/>
       <c r="G4" s="55" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="H4" s="27">
         <v>2</v>
@@ -1930,7 +1930,7 @@
         <v>92</v>
       </c>
       <c r="J4" s="44" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="K4" s="45" t="s">
         <v>69</v>
@@ -1943,7 +1943,7 @@
         <v>62</v>
       </c>
       <c r="O4" s="46" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="P4" s="65" t="s">
         <v>19</v>
@@ -1952,16 +1952,16 @@
         <v>6</v>
       </c>
       <c r="R4" s="49" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="S4" s="49" t="s">
+        <v>160</v>
+      </c>
+      <c r="T4" s="49" t="s">
+        <v>163</v>
+      </c>
+      <c r="U4" s="50" t="s">
         <v>162</v>
-      </c>
-      <c r="T4" s="49" t="s">
-        <v>165</v>
-      </c>
-      <c r="U4" s="50" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2002,7 +2002,7 @@
       </c>
       <c r="N5" s="9"/>
       <c r="O5" s="8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="P5" s="64" t="s">
         <v>19</v>
@@ -2011,16 +2011,16 @@
         <v>6</v>
       </c>
       <c r="R5" s="11" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="S5" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="T5" s="41" t="s">
+        <v>234</v>
+      </c>
+      <c r="U5" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="T5" s="41" t="s">
-        <v>236</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2061,7 +2061,7 @@
         <v>23</v>
       </c>
       <c r="O6" s="46" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="P6" s="63" t="s">
         <v>19</v>
@@ -2070,16 +2070,16 @@
         <v>6</v>
       </c>
       <c r="R6" s="11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="S6" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="T6" s="41" t="s">
+        <v>171</v>
+      </c>
+      <c r="U6" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="T6" s="41" t="s">
-        <v>173</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2111,7 +2111,7 @@
         <v>91</v>
       </c>
       <c r="J7" s="38" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="K7" s="40" t="s">
         <v>70</v>
@@ -2126,19 +2126,19 @@
         <v>19</v>
       </c>
       <c r="Q7" s="58" t="s">
+        <v>179</v>
+      </c>
+      <c r="R7" s="24" t="s">
+        <v>180</v>
+      </c>
+      <c r="S7" s="24" t="s">
         <v>181</v>
       </c>
-      <c r="R7" s="24" t="s">
+      <c r="T7" s="24" t="s">
         <v>182</v>
       </c>
-      <c r="S7" s="24" t="s">
+      <c r="U7" s="33" t="s">
         <v>183</v>
-      </c>
-      <c r="T7" s="24" t="s">
-        <v>184</v>
-      </c>
-      <c r="U7" s="33" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2183,7 +2183,7 @@
         <v>50</v>
       </c>
       <c r="O8" s="46" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="P8" s="61" t="s">
         <v>19</v>
@@ -2192,16 +2192,16 @@
         <v>6</v>
       </c>
       <c r="R8" s="24" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="S8" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="T8" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="U8" s="33" t="s">
         <v>162</v>
-      </c>
-      <c r="T8" s="24" t="s">
-        <v>176</v>
-      </c>
-      <c r="U8" s="33" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2246,7 +2246,7 @@
         <v>24</v>
       </c>
       <c r="O9" s="46" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="P9" s="61" t="s">
         <v>19</v>
@@ -2255,16 +2255,16 @@
         <v>6</v>
       </c>
       <c r="R9" s="24" t="s">
+        <v>159</v>
+      </c>
+      <c r="S9" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="T9" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="S9" s="24" t="s">
+      <c r="U9" s="33" t="s">
         <v>162</v>
-      </c>
-      <c r="T9" s="24" t="s">
-        <v>163</v>
-      </c>
-      <c r="U9" s="33" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2284,7 +2284,7 @@
         <v>114</v>
       </c>
       <c r="F10" s="35" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G10" s="55" t="s">
         <v>115</v>
@@ -2296,7 +2296,7 @@
         <v>92</v>
       </c>
       <c r="J10" s="38" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="K10" s="40" t="s">
         <v>69</v>
@@ -2309,7 +2309,7 @@
         <v>73</v>
       </c>
       <c r="O10" s="46" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="P10" s="61" t="s">
         <v>19</v>
@@ -2318,16 +2318,16 @@
         <v>6</v>
       </c>
       <c r="R10" s="11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="S10" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="T10" s="41" t="s">
+        <v>172</v>
+      </c>
+      <c r="U10" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="T10" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="U10" s="1" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2347,10 +2347,10 @@
         <v>114</v>
       </c>
       <c r="F11" s="35" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G11" s="57" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="H11" s="27">
         <v>9</v>
@@ -2359,7 +2359,7 @@
         <v>92</v>
       </c>
       <c r="J11" s="38" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="K11" s="40" t="s">
         <v>69</v>
@@ -2372,7 +2372,7 @@
         <v>61</v>
       </c>
       <c r="O11" s="46" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="P11" s="61" t="s">
         <v>20</v>
@@ -2381,16 +2381,16 @@
         <v>6</v>
       </c>
       <c r="R11" s="24" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="S11" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="T11" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="U11" s="33" t="s">
         <v>162</v>
-      </c>
-      <c r="T11" s="24" t="s">
-        <v>177</v>
-      </c>
-      <c r="U11" s="33" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2411,7 +2411,7 @@
       </c>
       <c r="F12" s="35"/>
       <c r="G12" s="37" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H12" s="27">
         <v>10</v>
@@ -2420,7 +2420,7 @@
         <v>92</v>
       </c>
       <c r="J12" s="38" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="K12" s="40" t="s">
         <v>69</v>
@@ -2442,16 +2442,16 @@
         <v>6</v>
       </c>
       <c r="R12" s="24" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="S12" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="T12" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="U12" s="33" t="s">
         <v>162</v>
-      </c>
-      <c r="T12" s="24" t="s">
-        <v>166</v>
-      </c>
-      <c r="U12" s="33" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2472,7 +2472,7 @@
       </c>
       <c r="F13" s="35"/>
       <c r="G13" s="37" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="H13" s="27">
         <v>11</v>
@@ -2494,7 +2494,7 @@
       </c>
       <c r="N13" s="9"/>
       <c r="O13" s="46" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="P13" s="61" t="s">
         <v>19</v>
@@ -2503,16 +2503,16 @@
         <v>6</v>
       </c>
       <c r="R13" s="25" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="S13" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="T13" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="U13" s="34" t="s">
         <v>156</v>
-      </c>
-      <c r="T13" s="25" t="s">
-        <v>159</v>
-      </c>
-      <c r="U13" s="34" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2555,7 +2555,7 @@
         <v>54</v>
       </c>
       <c r="O14" s="46" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="P14" s="61" t="s">
         <v>19</v>
@@ -2564,16 +2564,16 @@
         <v>6</v>
       </c>
       <c r="R14" s="25" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="S14" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="T14" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="U14" s="34" t="s">
         <v>162</v>
-      </c>
-      <c r="T14" s="25" t="s">
-        <v>175</v>
-      </c>
-      <c r="U14" s="34" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2603,7 +2603,7 @@
         <v>91</v>
       </c>
       <c r="J15" s="38" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="K15" s="40" t="s">
         <v>70</v>
@@ -2618,19 +2618,19 @@
         <v>19</v>
       </c>
       <c r="Q15" s="60" t="s">
+        <v>179</v>
+      </c>
+      <c r="R15" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="S15" s="25" t="s">
         <v>181</v>
-      </c>
-      <c r="R15" s="25" t="s">
-        <v>182</v>
-      </c>
-      <c r="S15" s="25" t="s">
-        <v>183</v>
       </c>
       <c r="T15" s="25" t="s">
         <v>122</v>
       </c>
       <c r="U15" s="34" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2651,7 +2651,7 @@
       </c>
       <c r="F16" s="35"/>
       <c r="G16" s="37" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H16" s="27">
         <v>14</v>
@@ -2675,19 +2675,19 @@
         <v>19</v>
       </c>
       <c r="Q16" s="59" t="s">
+        <v>179</v>
+      </c>
+      <c r="R16" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="S16" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="R16" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="S16" s="11" t="s">
+      <c r="T16" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="U16" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="T16" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="U16" s="1" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2708,7 +2708,7 @@
       </c>
       <c r="F17" s="35"/>
       <c r="G17" s="37" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H17" s="27">
         <v>15</v>
@@ -2730,7 +2730,7 @@
         <v>62</v>
       </c>
       <c r="O17" s="46" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="P17" s="61" t="s">
         <v>19</v>
@@ -2739,16 +2739,16 @@
         <v>6</v>
       </c>
       <c r="R17" s="11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="S17" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="T17" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="U17" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="T17" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="U17" s="1" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2791,7 +2791,7 @@
       </c>
       <c r="N18" s="9"/>
       <c r="O18" s="46" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="P18" s="61" t="s">
         <v>19</v>
@@ -2800,16 +2800,16 @@
         <v>6</v>
       </c>
       <c r="R18" s="11" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="S18" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="T18" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="U18" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="T18" s="11" t="s">
-        <v>240</v>
-      </c>
-      <c r="U18" s="1" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2852,7 +2852,7 @@
         <v>22</v>
       </c>
       <c r="O19" s="46" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="P19" s="61" t="s">
         <v>19</v>
@@ -2861,16 +2861,16 @@
         <v>6</v>
       </c>
       <c r="R19" s="11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="S19" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="T19" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="U19" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="T19" s="11" t="s">
-        <v>179</v>
-      </c>
-      <c r="U19" s="1" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2913,7 +2913,7 @@
       </c>
       <c r="N20" s="9"/>
       <c r="O20" s="46" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="P20" s="61" t="s">
         <v>19</v>
@@ -2922,16 +2922,16 @@
         <v>6</v>
       </c>
       <c r="R20" s="11" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="S20" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="T20" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="U20" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="T20" s="11" t="s">
-        <v>241</v>
-      </c>
-      <c r="U20" s="1" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2952,7 +2952,7 @@
       </c>
       <c r="F21" s="35"/>
       <c r="G21" s="37" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H21" s="27">
         <v>19</v>
@@ -2976,19 +2976,19 @@
         <v>19</v>
       </c>
       <c r="Q21" s="60" t="s">
+        <v>179</v>
+      </c>
+      <c r="R21" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="S21" s="25" t="s">
         <v>181</v>
       </c>
-      <c r="R21" s="25" t="s">
-        <v>182</v>
-      </c>
-      <c r="S21" s="25" t="s">
+      <c r="T21" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="U21" s="34" t="s">
         <v>183</v>
-      </c>
-      <c r="T21" s="25" t="s">
-        <v>187</v>
-      </c>
-      <c r="U21" s="34" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3020,7 +3020,7 @@
         <v>91</v>
       </c>
       <c r="J22" s="38" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="K22" s="40" t="s">
         <v>69</v>
@@ -3033,7 +3033,7 @@
       </c>
       <c r="N22" s="66"/>
       <c r="O22" s="8" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="P22" s="61" t="s">
         <v>19</v>
@@ -3042,16 +3042,16 @@
         <v>6</v>
       </c>
       <c r="R22" s="25" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="S22" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="T22" s="25" t="s">
+        <v>243</v>
+      </c>
+      <c r="U22" s="34" t="s">
         <v>156</v>
-      </c>
-      <c r="T22" s="25" t="s">
-        <v>245</v>
-      </c>
-      <c r="U22" s="34" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3105,16 +3105,16 @@
         <v>6</v>
       </c>
       <c r="R23" s="11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="S23" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="T23" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="U23" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="T23" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="U23" s="1" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3157,7 +3157,7 @@
       </c>
       <c r="N24" s="66"/>
       <c r="O24" s="8" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="P24" s="61" t="s">
         <v>19</v>
@@ -3166,16 +3166,16 @@
         <v>6</v>
       </c>
       <c r="R24" s="25" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="S24" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="T24" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="U24" s="34" t="s">
         <v>156</v>
-      </c>
-      <c r="T24" s="25" t="s">
-        <v>243</v>
-      </c>
-      <c r="U24" s="34" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="25" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3196,7 +3196,7 @@
       </c>
       <c r="F25" s="35"/>
       <c r="G25" s="37" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H25" s="27">
         <v>23</v>
@@ -3205,7 +3205,7 @@
         <v>92</v>
       </c>
       <c r="J25" s="38" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="K25" s="40" t="s">
         <v>69</v>
@@ -3218,7 +3218,7 @@
         <v>54</v>
       </c>
       <c r="O25" s="46" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="P25" s="61" t="s">
         <v>20</v>
@@ -3227,16 +3227,16 @@
         <v>6</v>
       </c>
       <c r="R25" s="25" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="S25" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="T25" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="U25" s="34" t="s">
         <v>162</v>
-      </c>
-      <c r="T25" s="25" t="s">
-        <v>217</v>
-      </c>
-      <c r="U25" s="34" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3257,7 +3257,7 @@
       </c>
       <c r="F26" s="35"/>
       <c r="G26" s="37" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="H26" s="27">
         <v>24</v>
@@ -3288,16 +3288,16 @@
         <v>6</v>
       </c>
       <c r="R26" s="25" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="S26" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="T26" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="U26" s="34" t="s">
         <v>162</v>
-      </c>
-      <c r="T26" s="25" t="s">
-        <v>167</v>
-      </c>
-      <c r="U26" s="34" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3318,7 +3318,7 @@
       </c>
       <c r="F27" s="35"/>
       <c r="G27" s="37" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="H27" s="27">
         <v>25</v>
@@ -3327,7 +3327,7 @@
         <v>92</v>
       </c>
       <c r="J27" s="38" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="K27" s="40" t="s">
         <v>70</v>
@@ -3344,19 +3344,19 @@
         <v>20</v>
       </c>
       <c r="Q27" s="58" t="s">
+        <v>179</v>
+      </c>
+      <c r="R27" s="24" t="s">
+        <v>180</v>
+      </c>
+      <c r="S27" s="24" t="s">
         <v>181</v>
       </c>
-      <c r="R27" s="24" t="s">
-        <v>182</v>
-      </c>
-      <c r="S27" s="24" t="s">
+      <c r="T27" s="24" t="s">
+        <v>206</v>
+      </c>
+      <c r="U27" s="33" t="s">
         <v>183</v>
-      </c>
-      <c r="T27" s="24" t="s">
-        <v>208</v>
-      </c>
-      <c r="U27" s="33" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="28" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3384,7 +3384,7 @@
         <v>91</v>
       </c>
       <c r="J28" s="38" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="K28" s="40" t="s">
         <v>69</v>
@@ -3406,16 +3406,16 @@
         <v>6</v>
       </c>
       <c r="R28" s="25" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="S28" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="T28" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="U28" s="34" t="s">
         <v>156</v>
-      </c>
-      <c r="T28" s="25" t="s">
-        <v>160</v>
-      </c>
-      <c r="U28" s="34" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="29" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3456,7 +3456,7 @@
         <v>73</v>
       </c>
       <c r="O29" s="46" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="P29" s="61" t="s">
         <v>19</v>
@@ -3465,16 +3465,16 @@
         <v>6</v>
       </c>
       <c r="R29" s="25" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="S29" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="T29" s="25" t="s">
+        <v>233</v>
+      </c>
+      <c r="U29" s="34" t="s">
         <v>162</v>
-      </c>
-      <c r="T29" s="25" t="s">
-        <v>235</v>
-      </c>
-      <c r="U29" s="34" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="30" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3495,7 +3495,7 @@
       </c>
       <c r="F30" s="35"/>
       <c r="G30" s="37" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H30" s="27">
         <v>28</v>
@@ -3504,7 +3504,7 @@
         <v>92</v>
       </c>
       <c r="J30" s="38" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="K30" s="40" t="s">
         <v>69</v>
@@ -3517,7 +3517,7 @@
         <v>62</v>
       </c>
       <c r="O30" s="8" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="P30" s="61" t="s">
         <v>19</v>
@@ -3526,16 +3526,16 @@
         <v>7</v>
       </c>
       <c r="R30" s="25" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="S30" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="T30" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="U30" s="34" t="s">
         <v>162</v>
-      </c>
-      <c r="T30" s="25" t="s">
-        <v>169</v>
-      </c>
-      <c r="U30" s="34" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="31" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3554,7 +3554,7 @@
       <c r="E31" s="26"/>
       <c r="F31" s="35"/>
       <c r="G31" s="37" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H31" s="27">
         <v>29</v>
@@ -3563,7 +3563,7 @@
         <v>92</v>
       </c>
       <c r="J31" s="38" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="K31" s="40" t="s">
         <v>69</v>
@@ -3576,7 +3576,7 @@
         <v>64</v>
       </c>
       <c r="O31" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="P31" s="61" t="s">
         <v>19</v>
@@ -3585,16 +3585,16 @@
         <v>10</v>
       </c>
       <c r="R31" s="25" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="S31" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="T31" s="25" t="s">
+        <v>168</v>
+      </c>
+      <c r="U31" s="34" t="s">
         <v>162</v>
-      </c>
-      <c r="T31" s="25" t="s">
-        <v>170</v>
-      </c>
-      <c r="U31" s="34" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="32" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3622,7 +3622,7 @@
         <v>92</v>
       </c>
       <c r="J32" s="38" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K32" s="40" t="s">
         <v>69</v>
@@ -3635,7 +3635,7 @@
         <v>64</v>
       </c>
       <c r="O32" s="46" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="P32" s="61" t="s">
         <v>19</v>
@@ -3644,16 +3644,16 @@
         <v>11</v>
       </c>
       <c r="R32" s="25" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="S32" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="T32" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="U32" s="34" t="s">
         <v>162</v>
-      </c>
-      <c r="T32" s="25" t="s">
-        <v>171</v>
-      </c>
-      <c r="U32" s="34" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="33" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3672,7 +3672,7 @@
       <c r="E33" s="26"/>
       <c r="F33" s="35"/>
       <c r="G33" s="37" t="s">
-        <v>147</v>
+        <v>248</v>
       </c>
       <c r="H33" s="27">
         <v>31</v>
@@ -3681,7 +3681,7 @@
         <v>92</v>
       </c>
       <c r="J33" s="38" t="s">
-        <v>149</v>
+        <v>249</v>
       </c>
       <c r="K33" s="40" t="s">
         <v>69</v>
@@ -3694,7 +3694,7 @@
         <v>64</v>
       </c>
       <c r="O33" s="46" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="P33" s="61" t="s">
         <v>19</v>
@@ -3703,16 +3703,16 @@
         <v>12</v>
       </c>
       <c r="R33" s="25" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="S33" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="T33" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="U33" s="34" t="s">
         <v>162</v>
-      </c>
-      <c r="T33" s="25" t="s">
-        <v>172</v>
-      </c>
-      <c r="U33" s="34" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="34" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3731,7 +3731,7 @@
       <c r="E34" s="26"/>
       <c r="F34" s="35"/>
       <c r="G34" s="37" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="H34" s="27">
         <v>32</v>
@@ -3740,7 +3740,7 @@
         <v>92</v>
       </c>
       <c r="J34" s="38" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="K34" s="40" t="s">
         <v>69</v>
@@ -3760,16 +3760,16 @@
         <v>6</v>
       </c>
       <c r="R34" s="11" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="S34" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="T34" s="41" t="s">
+        <v>247</v>
+      </c>
+      <c r="U34" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="T34" s="41" t="s">
-        <v>249</v>
-      </c>
-      <c r="U34" s="1" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="35" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3788,7 +3788,7 @@
       <c r="E35" s="26"/>
       <c r="F35" s="35"/>
       <c r="G35" s="37" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="H35" s="27">
         <v>33</v>
@@ -3797,7 +3797,7 @@
         <v>92</v>
       </c>
       <c r="J35" s="38" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="K35" s="40" t="s">
         <v>69</v>
@@ -3840,7 +3840,7 @@
         <v>92</v>
       </c>
       <c r="J36" s="38" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K36" s="40" t="s">
         <v>69</v>
@@ -3853,7 +3853,7 @@
         <v>23</v>
       </c>
       <c r="O36" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="P36" s="61" t="s">
         <v>19</v>
@@ -3862,16 +3862,16 @@
         <v>6</v>
       </c>
       <c r="R36" s="11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="S36" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="T36" s="41" t="s">
+        <v>176</v>
+      </c>
+      <c r="U36" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="T36" s="41" t="s">
-        <v>178</v>
-      </c>
-      <c r="U36" s="1" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
@@ -3890,7 +3890,7 @@
       <c r="E37" s="26"/>
       <c r="F37" s="35"/>
       <c r="G37" s="37" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="H37" s="27">
         <v>35</v>
@@ -3899,7 +3899,7 @@
         <v>92</v>
       </c>
       <c r="J37" s="38" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="K37" s="40" t="s">
         <v>69</v>
@@ -3919,16 +3919,16 @@
         <v>6</v>
       </c>
       <c r="R37" s="11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="S37" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="T37" s="41" t="s">
+        <v>202</v>
+      </c>
+      <c r="U37" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="T37" s="41" t="s">
-        <v>204</v>
-      </c>
-      <c r="U37" s="1" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
@@ -3936,11 +3936,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="M1:N1"/>
@@ -3956,6 +3951,11 @@
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Corrección de descripción de recurso
Se cambia animación por interactivo
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion01/ESCALETA_CN_09_01_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion01/ESCALETA_CN_09_01_CO.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="120" windowWidth="14370" windowHeight="11640"/>
@@ -11,7 +11,7 @@
     <sheet name="DATOS" sheetId="2" r:id="rId2"/>
     <sheet name="VER" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -380,9 +380,6 @@
     <t>La replicación del ADN</t>
   </si>
   <si>
-    <t>Animación que permite conocer el proceso de replicación del ADN y la maquinaria enzimática implicada</t>
-  </si>
-  <si>
     <t>Repasa el proceso de replicación</t>
   </si>
   <si>
@@ -772,6 +769,9 @@
   </si>
   <si>
     <t>Los estudiantes asocian el significado correspondiente, con los siguientes términos: cáncer, apoptosis, metástasis, oncogen, ciclo celular, mutación.</t>
+  </si>
+  <si>
+    <t>Interactivo que permite conocer el proceso de replicación del ADN y la maquinaria enzimática implicada</t>
   </si>
 </sst>
 </file>
@@ -1711,7 +1711,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1721,8 +1721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="O39" sqref="O39"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1856,10 +1856,10 @@
       </c>
       <c r="E3" s="30"/>
       <c r="F3" s="51" t="s">
+        <v>188</v>
+      </c>
+      <c r="G3" s="53" t="s">
         <v>189</v>
-      </c>
-      <c r="G3" s="53" t="s">
-        <v>190</v>
       </c>
       <c r="H3" s="31">
         <v>1</v>
@@ -1881,7 +1881,7 @@
       </c>
       <c r="N3" s="17"/>
       <c r="O3" s="16" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="P3" s="62" t="s">
         <v>19</v>
@@ -1890,16 +1890,16 @@
         <v>6</v>
       </c>
       <c r="R3" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="S3" s="19" t="s">
         <v>152</v>
       </c>
-      <c r="S3" s="19" t="s">
+      <c r="T3" s="19" t="s">
+        <v>240</v>
+      </c>
+      <c r="U3" s="20" t="s">
         <v>153</v>
-      </c>
-      <c r="T3" s="19" t="s">
-        <v>241</v>
-      </c>
-      <c r="U3" s="20" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1920,7 +1920,7 @@
       </c>
       <c r="F4" s="35"/>
       <c r="G4" s="55" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H4" s="27">
         <v>2</v>
@@ -1929,7 +1929,7 @@
         <v>92</v>
       </c>
       <c r="J4" s="44" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K4" s="45" t="s">
         <v>69</v>
@@ -1942,7 +1942,7 @@
         <v>62</v>
       </c>
       <c r="O4" s="46" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="P4" s="65" t="s">
         <v>19</v>
@@ -1951,16 +1951,16 @@
         <v>6</v>
       </c>
       <c r="R4" s="49" t="s">
+        <v>156</v>
+      </c>
+      <c r="S4" s="49" t="s">
         <v>157</v>
       </c>
-      <c r="S4" s="49" t="s">
-        <v>158</v>
-      </c>
       <c r="T4" s="49" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="U4" s="50" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2001,7 +2001,7 @@
       </c>
       <c r="N5" s="9"/>
       <c r="O5" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="P5" s="64" t="s">
         <v>19</v>
@@ -2010,16 +2010,16 @@
         <v>6</v>
       </c>
       <c r="R5" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="S5" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="S5" s="11" t="s">
+      <c r="T5" s="41" t="s">
+        <v>224</v>
+      </c>
+      <c r="U5" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="T5" s="41" t="s">
-        <v>225</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2060,7 +2060,7 @@
         <v>23</v>
       </c>
       <c r="O6" s="46" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="P6" s="63" t="s">
         <v>19</v>
@@ -2069,16 +2069,16 @@
         <v>6</v>
       </c>
       <c r="R6" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="S6" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="S6" s="11" t="s">
-        <v>158</v>
-      </c>
       <c r="T6" s="41" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2110,7 +2110,7 @@
         <v>91</v>
       </c>
       <c r="J7" s="38" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K7" s="40" t="s">
         <v>70</v>
@@ -2125,19 +2125,19 @@
         <v>19</v>
       </c>
       <c r="Q7" s="58" t="s">
+        <v>176</v>
+      </c>
+      <c r="R7" s="24" t="s">
         <v>177</v>
       </c>
-      <c r="R7" s="24" t="s">
+      <c r="S7" s="24" t="s">
         <v>178</v>
       </c>
-      <c r="S7" s="24" t="s">
+      <c r="T7" s="24" t="s">
         <v>179</v>
       </c>
-      <c r="T7" s="24" t="s">
+      <c r="U7" s="33" t="s">
         <v>180</v>
-      </c>
-      <c r="U7" s="33" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2182,7 +2182,7 @@
         <v>50</v>
       </c>
       <c r="O8" s="46" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="P8" s="61" t="s">
         <v>19</v>
@@ -2191,16 +2191,16 @@
         <v>6</v>
       </c>
       <c r="R8" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="S8" s="24" t="s">
         <v>157</v>
       </c>
-      <c r="S8" s="24" t="s">
-        <v>158</v>
-      </c>
       <c r="T8" s="24" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="U8" s="33" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2245,7 +2245,7 @@
         <v>24</v>
       </c>
       <c r="O9" s="46" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="P9" s="61" t="s">
         <v>19</v>
@@ -2254,16 +2254,16 @@
         <v>6</v>
       </c>
       <c r="R9" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="S9" s="24" t="s">
         <v>157</v>
       </c>
-      <c r="S9" s="24" t="s">
+      <c r="T9" s="24" t="s">
         <v>158</v>
       </c>
-      <c r="T9" s="24" t="s">
+      <c r="U9" s="33" t="s">
         <v>159</v>
-      </c>
-      <c r="U9" s="33" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2283,7 +2283,7 @@
         <v>114</v>
       </c>
       <c r="F10" s="35" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G10" s="55" t="s">
         <v>115</v>
@@ -2295,7 +2295,7 @@
         <v>92</v>
       </c>
       <c r="J10" s="38" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K10" s="40" t="s">
         <v>69</v>
@@ -2308,7 +2308,7 @@
         <v>73</v>
       </c>
       <c r="O10" s="46" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="P10" s="61" t="s">
         <v>19</v>
@@ -2317,16 +2317,16 @@
         <v>6</v>
       </c>
       <c r="R10" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="S10" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="S10" s="11" t="s">
-        <v>158</v>
-      </c>
       <c r="T10" s="41" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2346,10 +2346,10 @@
         <v>114</v>
       </c>
       <c r="F11" s="35" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G11" s="57" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H11" s="27">
         <v>9</v>
@@ -2358,7 +2358,7 @@
         <v>92</v>
       </c>
       <c r="J11" s="38" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K11" s="40" t="s">
         <v>69</v>
@@ -2371,7 +2371,7 @@
         <v>61</v>
       </c>
       <c r="O11" s="46" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="P11" s="61" t="s">
         <v>20</v>
@@ -2380,16 +2380,16 @@
         <v>6</v>
       </c>
       <c r="R11" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="S11" s="24" t="s">
         <v>157</v>
       </c>
-      <c r="S11" s="24" t="s">
-        <v>158</v>
-      </c>
       <c r="T11" s="24" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="U11" s="33" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2410,7 +2410,7 @@
       </c>
       <c r="F12" s="35"/>
       <c r="G12" s="37" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H12" s="27">
         <v>10</v>
@@ -2419,7 +2419,7 @@
         <v>92</v>
       </c>
       <c r="J12" s="38" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="K12" s="40" t="s">
         <v>69</v>
@@ -2441,16 +2441,16 @@
         <v>6</v>
       </c>
       <c r="R12" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="S12" s="24" t="s">
         <v>157</v>
       </c>
-      <c r="S12" s="24" t="s">
-        <v>158</v>
-      </c>
       <c r="T12" s="24" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="U12" s="33" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2471,7 +2471,7 @@
       </c>
       <c r="F13" s="35"/>
       <c r="G13" s="37" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H13" s="27">
         <v>11</v>
@@ -2480,7 +2480,7 @@
         <v>91</v>
       </c>
       <c r="J13" s="38" t="s">
-        <v>119</v>
+        <v>249</v>
       </c>
       <c r="K13" s="40" t="s">
         <v>69</v>
@@ -2493,7 +2493,7 @@
       </c>
       <c r="N13" s="9"/>
       <c r="O13" s="46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="P13" s="61" t="s">
         <v>19</v>
@@ -2502,16 +2502,16 @@
         <v>6</v>
       </c>
       <c r="R13" s="25" t="s">
+        <v>151</v>
+      </c>
+      <c r="S13" s="25" t="s">
         <v>152</v>
       </c>
-      <c r="S13" s="25" t="s">
+      <c r="T13" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="U13" s="34" t="s">
         <v>153</v>
-      </c>
-      <c r="T13" s="25" t="s">
-        <v>155</v>
-      </c>
-      <c r="U13" s="34" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2532,7 +2532,7 @@
       </c>
       <c r="F14" s="35"/>
       <c r="G14" s="37" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H14" s="27">
         <v>12</v>
@@ -2541,7 +2541,7 @@
         <v>92</v>
       </c>
       <c r="J14" s="38" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K14" s="40" t="s">
         <v>69</v>
@@ -2554,7 +2554,7 @@
         <v>54</v>
       </c>
       <c r="O14" s="46" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="P14" s="61" t="s">
         <v>19</v>
@@ -2563,16 +2563,16 @@
         <v>6</v>
       </c>
       <c r="R14" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="S14" s="25" t="s">
         <v>157</v>
       </c>
-      <c r="S14" s="25" t="s">
-        <v>158</v>
-      </c>
       <c r="T14" s="25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="U14" s="34" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2593,7 +2593,7 @@
       </c>
       <c r="F15" s="35"/>
       <c r="G15" s="37" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H15" s="27">
         <v>13</v>
@@ -2602,7 +2602,7 @@
         <v>91</v>
       </c>
       <c r="J15" s="38" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K15" s="40" t="s">
         <v>70</v>
@@ -2617,19 +2617,19 @@
         <v>19</v>
       </c>
       <c r="Q15" s="60" t="s">
+        <v>176</v>
+      </c>
+      <c r="R15" s="25" t="s">
         <v>177</v>
       </c>
-      <c r="R15" s="25" t="s">
+      <c r="S15" s="25" t="s">
         <v>178</v>
       </c>
-      <c r="S15" s="25" t="s">
-        <v>179</v>
-      </c>
       <c r="T15" s="25" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="U15" s="34" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2650,7 +2650,7 @@
       </c>
       <c r="F16" s="35"/>
       <c r="G16" s="37" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H16" s="27">
         <v>14</v>
@@ -2659,7 +2659,7 @@
         <v>92</v>
       </c>
       <c r="J16" s="38" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K16" s="40" t="s">
         <v>70</v>
@@ -2674,19 +2674,19 @@
         <v>19</v>
       </c>
       <c r="Q16" s="59" t="s">
+        <v>176</v>
+      </c>
+      <c r="R16" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="R16" s="11" t="s">
+      <c r="S16" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="S16" s="11" t="s">
-        <v>179</v>
-      </c>
       <c r="T16" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="U16" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2707,7 +2707,7 @@
       </c>
       <c r="F17" s="35"/>
       <c r="G17" s="37" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H17" s="27">
         <v>15</v>
@@ -2716,7 +2716,7 @@
         <v>92</v>
       </c>
       <c r="J17" s="38" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K17" s="40" t="s">
         <v>69</v>
@@ -2729,7 +2729,7 @@
         <v>62</v>
       </c>
       <c r="O17" s="46" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="P17" s="61" t="s">
         <v>19</v>
@@ -2738,16 +2738,16 @@
         <v>6</v>
       </c>
       <c r="R17" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="S17" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="S17" s="11" t="s">
-        <v>158</v>
-      </c>
       <c r="T17" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="U17" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2761,14 +2761,14 @@
         <v>97</v>
       </c>
       <c r="D18" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="E18" s="26" t="s">
         <v>125</v>
-      </c>
-      <c r="E18" s="26" t="s">
-        <v>126</v>
       </c>
       <c r="F18" s="35"/>
       <c r="G18" s="37" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H18" s="27">
         <v>16</v>
@@ -2777,7 +2777,7 @@
         <v>91</v>
       </c>
       <c r="J18" s="38" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K18" s="40" t="s">
         <v>69</v>
@@ -2790,7 +2790,7 @@
       </c>
       <c r="N18" s="9"/>
       <c r="O18" s="46" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="P18" s="61" t="s">
         <v>19</v>
@@ -2799,16 +2799,16 @@
         <v>6</v>
       </c>
       <c r="R18" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="S18" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="S18" s="11" t="s">
+      <c r="T18" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="U18" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="T18" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="U18" s="1" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2822,14 +2822,14 @@
         <v>97</v>
       </c>
       <c r="D19" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="E19" s="26" t="s">
         <v>125</v>
-      </c>
-      <c r="E19" s="26" t="s">
-        <v>126</v>
       </c>
       <c r="F19" s="35"/>
       <c r="G19" s="37" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H19" s="27">
         <v>17</v>
@@ -2838,7 +2838,7 @@
         <v>92</v>
       </c>
       <c r="J19" s="38" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K19" s="40" t="s">
         <v>69</v>
@@ -2851,7 +2851,7 @@
         <v>22</v>
       </c>
       <c r="O19" s="46" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="P19" s="61" t="s">
         <v>19</v>
@@ -2860,16 +2860,16 @@
         <v>6</v>
       </c>
       <c r="R19" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="S19" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="S19" s="11" t="s">
-        <v>158</v>
-      </c>
       <c r="T19" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="U19" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2883,14 +2883,14 @@
         <v>97</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E20" s="26" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F20" s="35"/>
       <c r="G20" s="37" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H20" s="27">
         <v>18</v>
@@ -2899,7 +2899,7 @@
         <v>91</v>
       </c>
       <c r="J20" s="38" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K20" s="40" t="s">
         <v>69</v>
@@ -2912,7 +2912,7 @@
       </c>
       <c r="N20" s="9"/>
       <c r="O20" s="46" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="P20" s="61" t="s">
         <v>19</v>
@@ -2921,16 +2921,16 @@
         <v>6</v>
       </c>
       <c r="R20" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="S20" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="S20" s="11" t="s">
+      <c r="T20" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="U20" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="T20" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="U20" s="1" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2944,14 +2944,14 @@
         <v>97</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E21" s="26" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F21" s="35"/>
       <c r="G21" s="37" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H21" s="27">
         <v>19</v>
@@ -2960,7 +2960,7 @@
         <v>92</v>
       </c>
       <c r="J21" s="38" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K21" s="40" t="s">
         <v>70</v>
@@ -2975,19 +2975,19 @@
         <v>19</v>
       </c>
       <c r="Q21" s="60" t="s">
+        <v>176</v>
+      </c>
+      <c r="R21" s="25" t="s">
         <v>177</v>
       </c>
-      <c r="R21" s="25" t="s">
+      <c r="S21" s="25" t="s">
         <v>178</v>
       </c>
-      <c r="S21" s="25" t="s">
-        <v>179</v>
-      </c>
       <c r="T21" s="25" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="U21" s="34" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3001,16 +3001,16 @@
         <v>97</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E22" s="26" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F22" s="35" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G22" s="37" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H22" s="27">
         <v>20</v>
@@ -3019,7 +3019,7 @@
         <v>91</v>
       </c>
       <c r="J22" s="38" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K22" s="40" t="s">
         <v>69</v>
@@ -3032,7 +3032,7 @@
       </c>
       <c r="N22" s="66"/>
       <c r="O22" s="8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="P22" s="61" t="s">
         <v>19</v>
@@ -3041,16 +3041,16 @@
         <v>6</v>
       </c>
       <c r="R22" s="25" t="s">
+        <v>151</v>
+      </c>
+      <c r="S22" s="25" t="s">
         <v>152</v>
       </c>
-      <c r="S22" s="25" t="s">
+      <c r="T22" s="25" t="s">
+        <v>232</v>
+      </c>
+      <c r="U22" s="34" t="s">
         <v>153</v>
-      </c>
-      <c r="T22" s="25" t="s">
-        <v>233</v>
-      </c>
-      <c r="U22" s="34" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="23" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3064,16 +3064,16 @@
         <v>97</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E23" s="26" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F23" s="35" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G23" s="37" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H23" s="27">
         <v>21</v>
@@ -3082,7 +3082,7 @@
         <v>92</v>
       </c>
       <c r="J23" s="38" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K23" s="40" t="s">
         <v>69</v>
@@ -3095,7 +3095,7 @@
         <v>74</v>
       </c>
       <c r="O23" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="P23" s="61" t="s">
         <v>19</v>
@@ -3104,16 +3104,16 @@
         <v>6</v>
       </c>
       <c r="R23" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="S23" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="S23" s="11" t="s">
-        <v>158</v>
-      </c>
       <c r="T23" s="11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="U23" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3127,14 +3127,14 @@
         <v>97</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E24" s="26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F24" s="35"/>
       <c r="G24" s="37" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H24" s="27">
         <v>22</v>
@@ -3143,7 +3143,7 @@
         <v>92</v>
       </c>
       <c r="J24" s="38" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K24" s="40" t="s">
         <v>69</v>
@@ -3156,7 +3156,7 @@
       </c>
       <c r="N24" s="66"/>
       <c r="O24" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P24" s="61" t="s">
         <v>19</v>
@@ -3165,16 +3165,16 @@
         <v>6</v>
       </c>
       <c r="R24" s="25" t="s">
+        <v>151</v>
+      </c>
+      <c r="S24" s="25" t="s">
         <v>152</v>
       </c>
-      <c r="S24" s="25" t="s">
+      <c r="T24" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="U24" s="34" t="s">
         <v>153</v>
-      </c>
-      <c r="T24" s="25" t="s">
-        <v>232</v>
-      </c>
-      <c r="U24" s="34" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="25" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3188,14 +3188,14 @@
         <v>97</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E25" s="26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F25" s="35"/>
       <c r="G25" s="37" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H25" s="27">
         <v>23</v>
@@ -3204,7 +3204,7 @@
         <v>92</v>
       </c>
       <c r="J25" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K25" s="40" t="s">
         <v>69</v>
@@ -3217,7 +3217,7 @@
         <v>54</v>
       </c>
       <c r="O25" s="46" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="P25" s="61" t="s">
         <v>20</v>
@@ -3226,16 +3226,16 @@
         <v>6</v>
       </c>
       <c r="R25" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="S25" s="25" t="s">
         <v>157</v>
       </c>
-      <c r="S25" s="25" t="s">
-        <v>158</v>
-      </c>
       <c r="T25" s="25" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="U25" s="34" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3249,14 +3249,14 @@
         <v>97</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E26" s="26" t="s">
         <v>100</v>
       </c>
       <c r="F26" s="35"/>
       <c r="G26" s="37" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H26" s="27">
         <v>24</v>
@@ -3265,7 +3265,7 @@
         <v>92</v>
       </c>
       <c r="J26" s="38" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K26" s="40" t="s">
         <v>69</v>
@@ -3278,7 +3278,7 @@
         <v>62</v>
       </c>
       <c r="O26" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="P26" s="61" t="s">
         <v>19</v>
@@ -3287,16 +3287,16 @@
         <v>6</v>
       </c>
       <c r="R26" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="S26" s="25" t="s">
         <v>157</v>
       </c>
-      <c r="S26" s="25" t="s">
-        <v>158</v>
-      </c>
       <c r="T26" s="25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="U26" s="34" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3310,14 +3310,14 @@
         <v>97</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E27" s="26" t="s">
         <v>100</v>
       </c>
       <c r="F27" s="35"/>
       <c r="G27" s="37" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H27" s="27">
         <v>25</v>
@@ -3326,7 +3326,7 @@
         <v>92</v>
       </c>
       <c r="J27" s="38" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K27" s="40" t="s">
         <v>70</v>
@@ -3343,19 +3343,19 @@
         <v>20</v>
       </c>
       <c r="Q27" s="58" t="s">
+        <v>176</v>
+      </c>
+      <c r="R27" s="24" t="s">
         <v>177</v>
       </c>
-      <c r="R27" s="24" t="s">
+      <c r="S27" s="24" t="s">
         <v>178</v>
       </c>
-      <c r="S27" s="24" t="s">
-        <v>179</v>
-      </c>
       <c r="T27" s="24" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="U27" s="33" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="28" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3369,12 +3369,12 @@
         <v>97</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E28" s="26"/>
       <c r="F28" s="35"/>
       <c r="G28" s="37" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H28" s="27">
         <v>26</v>
@@ -3383,7 +3383,7 @@
         <v>91</v>
       </c>
       <c r="J28" s="38" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K28" s="40" t="s">
         <v>69</v>
@@ -3396,7 +3396,7 @@
       </c>
       <c r="N28" s="9"/>
       <c r="O28" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="P28" s="61" t="s">
         <v>19</v>
@@ -3405,16 +3405,16 @@
         <v>6</v>
       </c>
       <c r="R28" s="25" t="s">
+        <v>151</v>
+      </c>
+      <c r="S28" s="25" t="s">
         <v>152</v>
       </c>
-      <c r="S28" s="25" t="s">
+      <c r="T28" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="U28" s="34" t="s">
         <v>153</v>
-      </c>
-      <c r="T28" s="25" t="s">
-        <v>156</v>
-      </c>
-      <c r="U28" s="34" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="29" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3428,12 +3428,12 @@
         <v>97</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E29" s="26"/>
       <c r="F29" s="35"/>
       <c r="G29" s="37" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H29" s="27">
         <v>27</v>
@@ -3442,7 +3442,7 @@
         <v>92</v>
       </c>
       <c r="J29" s="38" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K29" s="40" t="s">
         <v>69</v>
@@ -3455,7 +3455,7 @@
         <v>73</v>
       </c>
       <c r="O29" s="46" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="P29" s="61" t="s">
         <v>19</v>
@@ -3464,16 +3464,16 @@
         <v>6</v>
       </c>
       <c r="R29" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="S29" s="25" t="s">
         <v>157</v>
       </c>
-      <c r="S29" s="25" t="s">
-        <v>158</v>
-      </c>
       <c r="T29" s="25" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="U29" s="34" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="30" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3487,14 +3487,14 @@
         <v>97</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E30" s="26" t="s">
         <v>100</v>
       </c>
       <c r="F30" s="35"/>
       <c r="G30" s="37" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H30" s="27">
         <v>28</v>
@@ -3503,7 +3503,7 @@
         <v>92</v>
       </c>
       <c r="J30" s="38" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K30" s="40" t="s">
         <v>69</v>
@@ -3516,7 +3516,7 @@
         <v>62</v>
       </c>
       <c r="O30" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="P30" s="61" t="s">
         <v>19</v>
@@ -3525,16 +3525,16 @@
         <v>7</v>
       </c>
       <c r="R30" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="S30" s="25" t="s">
         <v>157</v>
       </c>
-      <c r="S30" s="25" t="s">
-        <v>158</v>
-      </c>
       <c r="T30" s="25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="U30" s="34" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="31" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3553,7 +3553,7 @@
       <c r="E31" s="26"/>
       <c r="F31" s="35"/>
       <c r="G31" s="37" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H31" s="27">
         <v>29</v>
@@ -3562,7 +3562,7 @@
         <v>92</v>
       </c>
       <c r="J31" s="38" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K31" s="40" t="s">
         <v>69</v>
@@ -3575,7 +3575,7 @@
         <v>64</v>
       </c>
       <c r="O31" s="46" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="P31" s="61" t="s">
         <v>19</v>
@@ -3584,16 +3584,16 @@
         <v>10</v>
       </c>
       <c r="R31" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="S31" s="25" t="s">
         <v>157</v>
       </c>
-      <c r="S31" s="25" t="s">
-        <v>158</v>
-      </c>
       <c r="T31" s="25" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="U31" s="34" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="32" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3612,7 +3612,7 @@
       <c r="E32" s="26"/>
       <c r="F32" s="35"/>
       <c r="G32" s="37" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H32" s="27">
         <v>30</v>
@@ -3621,7 +3621,7 @@
         <v>92</v>
       </c>
       <c r="J32" s="38" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K32" s="40" t="s">
         <v>69</v>
@@ -3634,7 +3634,7 @@
         <v>64</v>
       </c>
       <c r="O32" s="46" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="P32" s="61" t="s">
         <v>19</v>
@@ -3643,16 +3643,16 @@
         <v>11</v>
       </c>
       <c r="R32" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="S32" s="25" t="s">
         <v>157</v>
       </c>
-      <c r="S32" s="25" t="s">
-        <v>158</v>
-      </c>
       <c r="T32" s="25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="U32" s="34" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="33" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3671,7 +3671,7 @@
       <c r="E33" s="26"/>
       <c r="F33" s="35"/>
       <c r="G33" s="37" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H33" s="27">
         <v>31</v>
@@ -3680,7 +3680,7 @@
         <v>92</v>
       </c>
       <c r="J33" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K33" s="40" t="s">
         <v>69</v>
@@ -3693,7 +3693,7 @@
         <v>64</v>
       </c>
       <c r="O33" s="46" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="P33" s="61" t="s">
         <v>19</v>
@@ -3702,16 +3702,16 @@
         <v>12</v>
       </c>
       <c r="R33" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="S33" s="25" t="s">
         <v>157</v>
       </c>
-      <c r="S33" s="25" t="s">
-        <v>158</v>
-      </c>
       <c r="T33" s="25" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="U33" s="34" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="34" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3730,7 +3730,7 @@
       <c r="E34" s="26"/>
       <c r="F34" s="35"/>
       <c r="G34" s="37" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H34" s="27">
         <v>32</v>
@@ -3739,7 +3739,7 @@
         <v>92</v>
       </c>
       <c r="J34" s="38" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K34" s="40" t="s">
         <v>69</v>
@@ -3759,16 +3759,16 @@
         <v>6</v>
       </c>
       <c r="R34" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="S34" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="S34" s="11" t="s">
+      <c r="T34" s="41" t="s">
+        <v>236</v>
+      </c>
+      <c r="U34" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="T34" s="41" t="s">
-        <v>237</v>
-      </c>
-      <c r="U34" s="1" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="35" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3787,7 +3787,7 @@
       <c r="E35" s="26"/>
       <c r="F35" s="35"/>
       <c r="G35" s="37" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H35" s="27">
         <v>33</v>
@@ -3796,7 +3796,7 @@
         <v>92</v>
       </c>
       <c r="J35" s="38" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K35" s="40" t="s">
         <v>69</v>
@@ -3839,7 +3839,7 @@
         <v>92</v>
       </c>
       <c r="J36" s="38" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K36" s="40" t="s">
         <v>69</v>
@@ -3852,7 +3852,7 @@
         <v>23</v>
       </c>
       <c r="O36" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="P36" s="61" t="s">
         <v>19</v>
@@ -3861,16 +3861,16 @@
         <v>6</v>
       </c>
       <c r="R36" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="S36" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="S36" s="11" t="s">
-        <v>158</v>
-      </c>
       <c r="T36" s="41" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="U36" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
@@ -3889,7 +3889,7 @@
       <c r="E37" s="26"/>
       <c r="F37" s="35"/>
       <c r="G37" s="37" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H37" s="27">
         <v>35</v>
@@ -3898,7 +3898,7 @@
         <v>92</v>
       </c>
       <c r="J37" s="38" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K37" s="40" t="s">
         <v>69</v>
@@ -3918,16 +3918,16 @@
         <v>6</v>
       </c>
       <c r="R37" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="S37" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="S37" s="11" t="s">
-        <v>158</v>
-      </c>
       <c r="T37" s="41" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="U37" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
@@ -3935,11 +3935,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="M1:N1"/>
@@ -3955,6 +3950,11 @@
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Corrección código de motor
m15a por m14a
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion01/ESCALETA_CN_09_01_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion01/ESCALETA_CN_09_01_CO.xlsx
@@ -1711,7 +1711,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1722,7 +1722,7 @@
   <dimension ref="A1:U38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2368,7 +2368,7 @@
       </c>
       <c r="M11" s="66"/>
       <c r="N11" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O11" s="46" t="s">
         <v>212</v>
@@ -3935,6 +3935,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="M1:N1"/>
@@ -3950,11 +3955,6 @@
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Correcciones nombres secciones y recursos
Para que no coincidan secciones y recursos
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion01/ESCALETA_CN_09_01_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion01/ESCALETA_CN_09_01_CO.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="255">
   <si>
     <t>Asignatura</t>
   </si>
@@ -328,9 +328,6 @@
     <t>CN_09_01_CO</t>
   </si>
   <si>
-    <t>Nace una ciencia: la biología molecular</t>
-  </si>
-  <si>
     <t xml:space="preserve">Consolidación  </t>
   </si>
   <si>
@@ -442,13 +439,7 @@
     <t xml:space="preserve">La regulación genética  </t>
   </si>
   <si>
-    <t>Actividad acerca de la regulación genética</t>
-  </si>
-  <si>
     <t>Actividad de relacionar secuencias de codones con las secuencias de aminoácidos correspondientes (pueden ser todos imaginarios)</t>
-  </si>
-  <si>
-    <t>Una falla molecular: el cáncer</t>
   </si>
   <si>
     <t>Reconoce el significado de términos asociados al cáncer</t>
@@ -780,6 +771,30 @@
   </si>
   <si>
     <t>Las preguntas deben tener como mínimo las siguientes opciones de respuesta (que son las palabras del juego): ADN, ARN, proteína, enzima, nucleótido, aminoácido, base nitrogenada, uracilo.</t>
+  </si>
+  <si>
+    <t>Interactivo para comprender los aspectos básicos de la regulación genética</t>
+  </si>
+  <si>
+    <t>El nacimiento de una ciencia: la biología molecular</t>
+  </si>
+  <si>
+    <t>El cáncer, una falla molecular</t>
+  </si>
+  <si>
+    <t>Las moléculas de la herencia biológica</t>
+  </si>
+  <si>
+    <t>El proceso de traducción</t>
+  </si>
+  <si>
+    <t>El proceso de transcripción</t>
+  </si>
+  <si>
+    <t>¿Qué es el código genético?</t>
+  </si>
+  <si>
+    <t>Conoce la regulación genética</t>
   </si>
 </sst>
 </file>
@@ -1729,8 +1744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1860,14 +1875,14 @@
         <v>97</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>99</v>
+        <v>248</v>
       </c>
       <c r="E3" s="30"/>
       <c r="F3" s="51" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G3" s="53" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="H3" s="31">
         <v>1</v>
@@ -1876,7 +1891,7 @@
         <v>91</v>
       </c>
       <c r="J3" s="36" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K3" s="39" t="s">
         <v>69</v>
@@ -1889,7 +1904,7 @@
       </c>
       <c r="N3" s="17"/>
       <c r="O3" s="16" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="P3" s="62" t="s">
         <v>19</v>
@@ -1898,16 +1913,16 @@
         <v>6</v>
       </c>
       <c r="R3" s="19" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="S3" s="19" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="T3" s="19" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="U3" s="20" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1921,14 +1936,14 @@
         <v>97</v>
       </c>
       <c r="D4" s="29" t="s">
+        <v>248</v>
+      </c>
+      <c r="E4" s="26" t="s">
         <v>99</v>
-      </c>
-      <c r="E4" s="26" t="s">
-        <v>100</v>
       </c>
       <c r="F4" s="35"/>
       <c r="G4" s="55" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="H4" s="27">
         <v>2</v>
@@ -1937,7 +1952,7 @@
         <v>92</v>
       </c>
       <c r="J4" s="44" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="K4" s="45" t="s">
         <v>69</v>
@@ -1950,7 +1965,7 @@
         <v>62</v>
       </c>
       <c r="O4" s="46" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="P4" s="65" t="s">
         <v>19</v>
@@ -1959,16 +1974,16 @@
         <v>6</v>
       </c>
       <c r="R4" s="49" t="s">
+        <v>153</v>
+      </c>
+      <c r="S4" s="49" t="s">
+        <v>154</v>
+      </c>
+      <c r="T4" s="49" t="s">
+        <v>157</v>
+      </c>
+      <c r="U4" s="50" t="s">
         <v>156</v>
-      </c>
-      <c r="S4" s="49" t="s">
-        <v>157</v>
-      </c>
-      <c r="T4" s="49" t="s">
-        <v>160</v>
-      </c>
-      <c r="U4" s="50" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1982,12 +1997,12 @@
         <v>97</v>
       </c>
       <c r="D5" s="54" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E5" s="26"/>
       <c r="F5" s="52"/>
       <c r="G5" s="37" t="s">
-        <v>101</v>
+        <v>250</v>
       </c>
       <c r="H5" s="27">
         <v>3</v>
@@ -1996,7 +2011,7 @@
         <v>91</v>
       </c>
       <c r="J5" s="38" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K5" s="40" t="s">
         <v>69</v>
@@ -2009,7 +2024,7 @@
       </c>
       <c r="N5" s="9"/>
       <c r="O5" s="8" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="P5" s="64" t="s">
         <v>19</v>
@@ -2018,16 +2033,16 @@
         <v>6</v>
       </c>
       <c r="R5" s="11" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="S5" s="11" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="T5" s="41" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2041,12 +2056,12 @@
         <v>97</v>
       </c>
       <c r="D6" s="54" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E6" s="26"/>
       <c r="F6" s="35"/>
       <c r="G6" s="37" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H6" s="27">
         <v>4</v>
@@ -2055,7 +2070,7 @@
         <v>92</v>
       </c>
       <c r="J6" s="38" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K6" s="40" t="s">
         <v>69</v>
@@ -2068,7 +2083,7 @@
         <v>23</v>
       </c>
       <c r="O6" s="46" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="P6" s="63" t="s">
         <v>19</v>
@@ -2077,16 +2092,16 @@
         <v>6</v>
       </c>
       <c r="R6" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="S6" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="T6" s="41" t="s">
+        <v>165</v>
+      </c>
+      <c r="U6" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="S6" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="T6" s="41" t="s">
-        <v>168</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2100,16 +2115,16 @@
         <v>97</v>
       </c>
       <c r="D7" s="54" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E7" s="26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F7" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="G7" s="37" t="s">
         <v>107</v>
-      </c>
-      <c r="G7" s="37" t="s">
-        <v>108</v>
       </c>
       <c r="H7" s="27">
         <v>5</v>
@@ -2118,7 +2133,7 @@
         <v>91</v>
       </c>
       <c r="J7" s="38" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="K7" s="40" t="s">
         <v>70</v>
@@ -2133,19 +2148,19 @@
         <v>19</v>
       </c>
       <c r="Q7" s="58" t="s">
+        <v>172</v>
+      </c>
+      <c r="R7" s="24" t="s">
+        <v>173</v>
+      </c>
+      <c r="S7" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="T7" s="24" t="s">
         <v>175</v>
       </c>
-      <c r="R7" s="24" t="s">
+      <c r="U7" s="33" t="s">
         <v>176</v>
-      </c>
-      <c r="S7" s="24" t="s">
-        <v>177</v>
-      </c>
-      <c r="T7" s="24" t="s">
-        <v>178</v>
-      </c>
-      <c r="U7" s="33" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2159,16 +2174,16 @@
         <v>97</v>
       </c>
       <c r="D8" s="54" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F8" s="35" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G8" s="37" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H8" s="27">
         <v>6</v>
@@ -2177,7 +2192,7 @@
         <v>92</v>
       </c>
       <c r="J8" s="38" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K8" s="40" t="s">
         <v>69</v>
@@ -2190,7 +2205,7 @@
         <v>50</v>
       </c>
       <c r="O8" s="46" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="P8" s="61" t="s">
         <v>19</v>
@@ -2199,16 +2214,16 @@
         <v>6</v>
       </c>
       <c r="R8" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="S8" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="T8" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="U8" s="33" t="s">
         <v>156</v>
-      </c>
-      <c r="S8" s="24" t="s">
-        <v>157</v>
-      </c>
-      <c r="T8" s="24" t="s">
-        <v>171</v>
-      </c>
-      <c r="U8" s="33" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2222,16 +2237,16 @@
         <v>97</v>
       </c>
       <c r="D9" s="54" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F9" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="G9" s="56" t="s">
         <v>111</v>
-      </c>
-      <c r="G9" s="56" t="s">
-        <v>112</v>
       </c>
       <c r="H9" s="27">
         <v>7</v>
@@ -2240,7 +2255,7 @@
         <v>92</v>
       </c>
       <c r="J9" s="38" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K9" s="40" t="s">
         <v>69</v>
@@ -2253,7 +2268,7 @@
         <v>24</v>
       </c>
       <c r="O9" s="46" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="P9" s="61" t="s">
         <v>19</v>
@@ -2262,16 +2277,16 @@
         <v>6</v>
       </c>
       <c r="R9" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="S9" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="T9" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="U9" s="33" t="s">
         <v>156</v>
-      </c>
-      <c r="S9" s="24" t="s">
-        <v>157</v>
-      </c>
-      <c r="T9" s="24" t="s">
-        <v>158</v>
-      </c>
-      <c r="U9" s="33" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2285,16 +2300,16 @@
         <v>97</v>
       </c>
       <c r="D10" s="54" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E10" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="F10" s="35" t="s">
+        <v>227</v>
+      </c>
+      <c r="G10" s="55" t="s">
         <v>114</v>
-      </c>
-      <c r="F10" s="35" t="s">
-        <v>230</v>
-      </c>
-      <c r="G10" s="55" t="s">
-        <v>115</v>
       </c>
       <c r="H10" s="27">
         <v>8</v>
@@ -2303,7 +2318,7 @@
         <v>92</v>
       </c>
       <c r="J10" s="38" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K10" s="40" t="s">
         <v>69</v>
@@ -2316,7 +2331,7 @@
         <v>73</v>
       </c>
       <c r="O10" s="46" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="P10" s="61" t="s">
         <v>19</v>
@@ -2325,16 +2340,16 @@
         <v>6</v>
       </c>
       <c r="R10" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="S10" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="T10" s="41" t="s">
+        <v>166</v>
+      </c>
+      <c r="U10" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="S10" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="T10" s="41" t="s">
-        <v>169</v>
-      </c>
-      <c r="U10" s="1" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2348,16 +2363,16 @@
         <v>97</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F11" s="35" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="G11" s="57" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="H11" s="27">
         <v>9</v>
@@ -2366,7 +2381,7 @@
         <v>92</v>
       </c>
       <c r="J11" s="38" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="K11" s="40" t="s">
         <v>69</v>
@@ -2379,7 +2394,7 @@
         <v>60</v>
       </c>
       <c r="O11" s="46" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="P11" s="61" t="s">
         <v>20</v>
@@ -2388,16 +2403,16 @@
         <v>6</v>
       </c>
       <c r="R11" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="S11" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="T11" s="24" t="s">
+        <v>244</v>
+      </c>
+      <c r="U11" s="33" t="s">
         <v>156</v>
-      </c>
-      <c r="S11" s="24" t="s">
-        <v>157</v>
-      </c>
-      <c r="T11" s="24" t="s">
-        <v>247</v>
-      </c>
-      <c r="U11" s="33" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2411,14 +2426,14 @@
         <v>97</v>
       </c>
       <c r="D12" s="54" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E12" s="26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F12" s="35"/>
       <c r="G12" s="37" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="H12" s="27">
         <v>10</v>
@@ -2427,7 +2442,7 @@
         <v>92</v>
       </c>
       <c r="J12" s="38" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="K12" s="40" t="s">
         <v>69</v>
@@ -2440,7 +2455,7 @@
         <v>62</v>
       </c>
       <c r="O12" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="P12" s="61" t="s">
         <v>19</v>
@@ -2449,16 +2464,16 @@
         <v>6</v>
       </c>
       <c r="R12" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="S12" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="T12" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="U12" s="33" t="s">
         <v>156</v>
-      </c>
-      <c r="S12" s="24" t="s">
-        <v>157</v>
-      </c>
-      <c r="T12" s="24" t="s">
-        <v>161</v>
-      </c>
-      <c r="U12" s="33" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2472,14 +2487,14 @@
         <v>97</v>
       </c>
       <c r="D13" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="E13" s="26" t="s">
         <v>117</v>
-      </c>
-      <c r="E13" s="26" t="s">
-        <v>118</v>
       </c>
       <c r="F13" s="35"/>
       <c r="G13" s="37" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="H13" s="27">
         <v>11</v>
@@ -2488,7 +2503,7 @@
         <v>91</v>
       </c>
       <c r="J13" s="38" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="K13" s="40" t="s">
         <v>69</v>
@@ -2501,7 +2516,7 @@
       </c>
       <c r="N13" s="9"/>
       <c r="O13" s="46" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="P13" s="61" t="s">
         <v>19</v>
@@ -2510,16 +2525,16 @@
         <v>6</v>
       </c>
       <c r="R13" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="S13" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="T13" s="25" t="s">
         <v>151</v>
       </c>
-      <c r="S13" s="25" t="s">
-        <v>152</v>
-      </c>
-      <c r="T13" s="25" t="s">
-        <v>154</v>
-      </c>
       <c r="U13" s="34" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2533,14 +2548,14 @@
         <v>97</v>
       </c>
       <c r="D14" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="E14" s="26" t="s">
         <v>117</v>
-      </c>
-      <c r="E14" s="26" t="s">
-        <v>118</v>
       </c>
       <c r="F14" s="35"/>
       <c r="G14" s="37" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H14" s="27">
         <v>12</v>
@@ -2549,7 +2564,7 @@
         <v>92</v>
       </c>
       <c r="J14" s="38" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K14" s="40" t="s">
         <v>69</v>
@@ -2562,7 +2577,7 @@
         <v>54</v>
       </c>
       <c r="O14" s="46" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="P14" s="61" t="s">
         <v>19</v>
@@ -2571,16 +2586,16 @@
         <v>6</v>
       </c>
       <c r="R14" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="S14" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="T14" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="U14" s="34" t="s">
         <v>156</v>
-      </c>
-      <c r="S14" s="25" t="s">
-        <v>157</v>
-      </c>
-      <c r="T14" s="25" t="s">
-        <v>170</v>
-      </c>
-      <c r="U14" s="34" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2594,14 +2609,14 @@
         <v>97</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E15" s="26" t="s">
         <v>96</v>
       </c>
       <c r="F15" s="35"/>
       <c r="G15" s="37" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H15" s="27">
         <v>13</v>
@@ -2610,7 +2625,7 @@
         <v>91</v>
       </c>
       <c r="J15" s="38" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="K15" s="40" t="s">
         <v>70</v>
@@ -2625,19 +2640,19 @@
         <v>19</v>
       </c>
       <c r="Q15" s="60" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="R15" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="S15" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="T15" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="U15" s="34" t="s">
         <v>176</v>
-      </c>
-      <c r="S15" s="25" t="s">
-        <v>177</v>
-      </c>
-      <c r="T15" s="25" t="s">
-        <v>121</v>
-      </c>
-      <c r="U15" s="34" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2651,14 +2666,14 @@
         <v>97</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E16" s="26" t="s">
         <v>96</v>
       </c>
       <c r="F16" s="35"/>
       <c r="G16" s="37" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="H16" s="27">
         <v>14</v>
@@ -2667,7 +2682,7 @@
         <v>92</v>
       </c>
       <c r="J16" s="38" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K16" s="40" t="s">
         <v>70</v>
@@ -2682,19 +2697,19 @@
         <v>19</v>
       </c>
       <c r="Q16" s="59" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="R16" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="S16" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="T16" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="U16" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="S16" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="T16" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="U16" s="1" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2708,14 +2723,14 @@
         <v>97</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E17" s="26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F17" s="35"/>
       <c r="G17" s="37" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="H17" s="27">
         <v>15</v>
@@ -2724,7 +2739,7 @@
         <v>92</v>
       </c>
       <c r="J17" s="38" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K17" s="40" t="s">
         <v>69</v>
@@ -2737,7 +2752,7 @@
         <v>62</v>
       </c>
       <c r="O17" s="46" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="P17" s="61" t="s">
         <v>19</v>
@@ -2746,16 +2761,16 @@
         <v>6</v>
       </c>
       <c r="R17" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="S17" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="T17" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="U17" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="S17" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="T17" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="U17" s="1" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2769,14 +2784,14 @@
         <v>97</v>
       </c>
       <c r="D18" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="E18" s="26" t="s">
         <v>124</v>
-      </c>
-      <c r="E18" s="26" t="s">
-        <v>125</v>
       </c>
       <c r="F18" s="35"/>
       <c r="G18" s="37" t="s">
-        <v>125</v>
+        <v>252</v>
       </c>
       <c r="H18" s="27">
         <v>16</v>
@@ -2785,7 +2800,7 @@
         <v>91</v>
       </c>
       <c r="J18" s="38" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K18" s="40" t="s">
         <v>69</v>
@@ -2798,7 +2813,7 @@
       </c>
       <c r="N18" s="9"/>
       <c r="O18" s="46" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="P18" s="61" t="s">
         <v>19</v>
@@ -2807,16 +2822,16 @@
         <v>6</v>
       </c>
       <c r="R18" s="11" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="S18" s="11" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="T18" s="11" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="U18" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2830,14 +2845,14 @@
         <v>97</v>
       </c>
       <c r="D19" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="E19" s="26" t="s">
         <v>124</v>
-      </c>
-      <c r="E19" s="26" t="s">
-        <v>125</v>
       </c>
       <c r="F19" s="35"/>
       <c r="G19" s="37" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H19" s="27">
         <v>17</v>
@@ -2846,7 +2861,7 @@
         <v>92</v>
       </c>
       <c r="J19" s="38" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K19" s="40" t="s">
         <v>69</v>
@@ -2859,7 +2874,7 @@
         <v>22</v>
       </c>
       <c r="O19" s="46" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="P19" s="61" t="s">
         <v>19</v>
@@ -2868,16 +2883,16 @@
         <v>6</v>
       </c>
       <c r="R19" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="S19" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="T19" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="U19" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="S19" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="T19" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="U19" s="1" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2891,14 +2906,14 @@
         <v>97</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E20" s="26" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F20" s="35"/>
       <c r="G20" s="37" t="s">
-        <v>126</v>
+        <v>251</v>
       </c>
       <c r="H20" s="27">
         <v>18</v>
@@ -2907,7 +2922,7 @@
         <v>91</v>
       </c>
       <c r="J20" s="38" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K20" s="40" t="s">
         <v>69</v>
@@ -2920,7 +2935,7 @@
       </c>
       <c r="N20" s="9"/>
       <c r="O20" s="46" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="P20" s="61" t="s">
         <v>19</v>
@@ -2929,16 +2944,16 @@
         <v>6</v>
       </c>
       <c r="R20" s="11" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="S20" s="11" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="T20" s="11" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="U20" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2952,14 +2967,14 @@
         <v>97</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E21" s="26" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F21" s="35"/>
       <c r="G21" s="37" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="H21" s="27">
         <v>19</v>
@@ -2968,7 +2983,7 @@
         <v>92</v>
       </c>
       <c r="J21" s="38" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K21" s="40" t="s">
         <v>70</v>
@@ -2983,19 +2998,19 @@
         <v>19</v>
       </c>
       <c r="Q21" s="60" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="R21" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="S21" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="T21" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="U21" s="34" t="s">
         <v>176</v>
-      </c>
-      <c r="S21" s="25" t="s">
-        <v>177</v>
-      </c>
-      <c r="T21" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="U21" s="34" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3009,16 +3024,16 @@
         <v>97</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E22" s="26" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F22" s="35" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G22" s="37" t="s">
-        <v>129</v>
+        <v>253</v>
       </c>
       <c r="H22" s="27">
         <v>20</v>
@@ -3027,7 +3042,7 @@
         <v>91</v>
       </c>
       <c r="J22" s="38" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="K22" s="40" t="s">
         <v>69</v>
@@ -3040,7 +3055,7 @@
       </c>
       <c r="N22" s="66"/>
       <c r="O22" s="8" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="P22" s="61" t="s">
         <v>19</v>
@@ -3049,16 +3064,16 @@
         <v>6</v>
       </c>
       <c r="R22" s="25" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="S22" s="25" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="T22" s="25" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="U22" s="34" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="23" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3072,16 +3087,16 @@
         <v>97</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E23" s="26" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F23" s="35" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G23" s="37" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H23" s="27">
         <v>21</v>
@@ -3090,7 +3105,7 @@
         <v>92</v>
       </c>
       <c r="J23" s="38" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K23" s="40" t="s">
         <v>69</v>
@@ -3103,7 +3118,7 @@
         <v>74</v>
       </c>
       <c r="O23" s="8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="P23" s="61" t="s">
         <v>19</v>
@@ -3112,16 +3127,16 @@
         <v>6</v>
       </c>
       <c r="R23" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="S23" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="T23" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="U23" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="S23" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="T23" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="U23" s="1" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3135,14 +3150,14 @@
         <v>97</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E24" s="26" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F24" s="35"/>
       <c r="G24" s="37" t="s">
-        <v>136</v>
+        <v>254</v>
       </c>
       <c r="H24" s="27">
         <v>22</v>
@@ -3151,7 +3166,7 @@
         <v>91</v>
       </c>
       <c r="J24" s="38" t="s">
-        <v>137</v>
+        <v>247</v>
       </c>
       <c r="K24" s="40" t="s">
         <v>69</v>
@@ -3164,7 +3179,7 @@
       </c>
       <c r="N24" s="66"/>
       <c r="O24" s="8" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="P24" s="61" t="s">
         <v>19</v>
@@ -3173,16 +3188,16 @@
         <v>6</v>
       </c>
       <c r="R24" s="25" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="S24" s="25" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="T24" s="25" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="U24" s="34" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="25" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3196,14 +3211,14 @@
         <v>97</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E25" s="26" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F25" s="35"/>
       <c r="G25" s="37" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="H25" s="27">
         <v>23</v>
@@ -3212,7 +3227,7 @@
         <v>92</v>
       </c>
       <c r="J25" s="38" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="K25" s="40" t="s">
         <v>69</v>
@@ -3225,7 +3240,7 @@
         <v>54</v>
       </c>
       <c r="O25" s="46" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="P25" s="61" t="s">
         <v>20</v>
@@ -3234,16 +3249,16 @@
         <v>6</v>
       </c>
       <c r="R25" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="S25" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="T25" s="25" t="s">
+        <v>203</v>
+      </c>
+      <c r="U25" s="34" t="s">
         <v>156</v>
-      </c>
-      <c r="S25" s="25" t="s">
-        <v>157</v>
-      </c>
-      <c r="T25" s="25" t="s">
-        <v>206</v>
-      </c>
-      <c r="U25" s="34" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3257,14 +3272,14 @@
         <v>97</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E26" s="26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F26" s="35"/>
       <c r="G26" s="37" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="H26" s="27">
         <v>24</v>
@@ -3273,7 +3288,7 @@
         <v>92</v>
       </c>
       <c r="J26" s="38" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K26" s="40" t="s">
         <v>69</v>
@@ -3286,7 +3301,7 @@
         <v>62</v>
       </c>
       <c r="O26" s="8" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="P26" s="61" t="s">
         <v>19</v>
@@ -3295,16 +3310,16 @@
         <v>6</v>
       </c>
       <c r="R26" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="S26" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="T26" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="U26" s="34" t="s">
         <v>156</v>
-      </c>
-      <c r="S26" s="25" t="s">
-        <v>157</v>
-      </c>
-      <c r="T26" s="25" t="s">
-        <v>162</v>
-      </c>
-      <c r="U26" s="34" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3318,14 +3333,14 @@
         <v>97</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E27" s="26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F27" s="35"/>
       <c r="G27" s="37" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="H27" s="27">
         <v>25</v>
@@ -3334,7 +3349,7 @@
         <v>92</v>
       </c>
       <c r="J27" s="38" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="K27" s="40" t="s">
         <v>70</v>
@@ -3351,19 +3366,19 @@
         <v>20</v>
       </c>
       <c r="Q27" s="58" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="R27" s="24" t="s">
+        <v>173</v>
+      </c>
+      <c r="S27" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="T27" s="24" t="s">
+        <v>198</v>
+      </c>
+      <c r="U27" s="33" t="s">
         <v>176</v>
-      </c>
-      <c r="S27" s="24" t="s">
-        <v>177</v>
-      </c>
-      <c r="T27" s="24" t="s">
-        <v>201</v>
-      </c>
-      <c r="U27" s="33" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="28" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3377,12 +3392,12 @@
         <v>97</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>139</v>
+        <v>249</v>
       </c>
       <c r="E28" s="26"/>
       <c r="F28" s="35"/>
       <c r="G28" s="37" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H28" s="27">
         <v>26</v>
@@ -3391,7 +3406,7 @@
         <v>91</v>
       </c>
       <c r="J28" s="38" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="K28" s="40" t="s">
         <v>69</v>
@@ -3404,7 +3419,7 @@
       </c>
       <c r="N28" s="9"/>
       <c r="O28" s="8" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="P28" s="61" t="s">
         <v>19</v>
@@ -3413,16 +3428,16 @@
         <v>6</v>
       </c>
       <c r="R28" s="25" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="S28" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="T28" s="25" t="s">
         <v>152</v>
       </c>
-      <c r="T28" s="25" t="s">
-        <v>155</v>
-      </c>
       <c r="U28" s="34" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="29" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3436,12 +3451,12 @@
         <v>97</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>139</v>
+        <v>249</v>
       </c>
       <c r="E29" s="26"/>
       <c r="F29" s="35"/>
       <c r="G29" s="37" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="H29" s="27">
         <v>27</v>
@@ -3450,7 +3465,7 @@
         <v>92</v>
       </c>
       <c r="J29" s="38" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="K29" s="40" t="s">
         <v>69</v>
@@ -3463,7 +3478,7 @@
         <v>73</v>
       </c>
       <c r="O29" s="46" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="P29" s="61" t="s">
         <v>19</v>
@@ -3472,16 +3487,16 @@
         <v>6</v>
       </c>
       <c r="R29" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="S29" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="T29" s="25" t="s">
+        <v>217</v>
+      </c>
+      <c r="U29" s="34" t="s">
         <v>156</v>
-      </c>
-      <c r="S29" s="25" t="s">
-        <v>157</v>
-      </c>
-      <c r="T29" s="25" t="s">
-        <v>220</v>
-      </c>
-      <c r="U29" s="34" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="30" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3495,14 +3510,14 @@
         <v>97</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>139</v>
+        <v>249</v>
       </c>
       <c r="E30" s="26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F30" s="35"/>
       <c r="G30" s="37" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="H30" s="27">
         <v>28</v>
@@ -3511,7 +3526,7 @@
         <v>92</v>
       </c>
       <c r="J30" s="38" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="K30" s="40" t="s">
         <v>69</v>
@@ -3524,7 +3539,7 @@
         <v>62</v>
       </c>
       <c r="O30" s="8" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="P30" s="61" t="s">
         <v>19</v>
@@ -3533,16 +3548,16 @@
         <v>7</v>
       </c>
       <c r="R30" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="S30" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="T30" s="25" t="s">
+        <v>161</v>
+      </c>
+      <c r="U30" s="34" t="s">
         <v>156</v>
-      </c>
-      <c r="S30" s="25" t="s">
-        <v>157</v>
-      </c>
-      <c r="T30" s="25" t="s">
-        <v>164</v>
-      </c>
-      <c r="U30" s="34" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="31" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3561,7 +3576,7 @@
       <c r="E31" s="26"/>
       <c r="F31" s="35"/>
       <c r="G31" s="37" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H31" s="27">
         <v>29</v>
@@ -3570,7 +3585,7 @@
         <v>92</v>
       </c>
       <c r="J31" s="38" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="K31" s="40" t="s">
         <v>69</v>
@@ -3583,7 +3598,7 @@
         <v>64</v>
       </c>
       <c r="O31" s="46" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="P31" s="61" t="s">
         <v>19</v>
@@ -3592,16 +3607,16 @@
         <v>10</v>
       </c>
       <c r="R31" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="S31" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="T31" s="25" t="s">
+        <v>162</v>
+      </c>
+      <c r="U31" s="34" t="s">
         <v>156</v>
-      </c>
-      <c r="S31" s="25" t="s">
-        <v>157</v>
-      </c>
-      <c r="T31" s="25" t="s">
-        <v>165</v>
-      </c>
-      <c r="U31" s="34" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="32" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3620,7 +3635,7 @@
       <c r="E32" s="26"/>
       <c r="F32" s="35"/>
       <c r="G32" s="37" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="H32" s="27">
         <v>30</v>
@@ -3629,7 +3644,7 @@
         <v>92</v>
       </c>
       <c r="J32" s="38" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="K32" s="40" t="s">
         <v>69</v>
@@ -3642,7 +3657,7 @@
         <v>64</v>
       </c>
       <c r="O32" s="46" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="P32" s="61" t="s">
         <v>19</v>
@@ -3651,16 +3666,16 @@
         <v>11</v>
       </c>
       <c r="R32" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="S32" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="T32" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="U32" s="34" t="s">
         <v>156</v>
-      </c>
-      <c r="S32" s="25" t="s">
-        <v>157</v>
-      </c>
-      <c r="T32" s="25" t="s">
-        <v>166</v>
-      </c>
-      <c r="U32" s="34" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="33" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3679,7 +3694,7 @@
       <c r="E33" s="26"/>
       <c r="F33" s="35"/>
       <c r="G33" s="37" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="H33" s="27">
         <v>31</v>
@@ -3688,7 +3703,7 @@
         <v>92</v>
       </c>
       <c r="J33" s="38" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="K33" s="40" t="s">
         <v>69</v>
@@ -3701,7 +3716,7 @@
         <v>64</v>
       </c>
       <c r="O33" s="46" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="P33" s="61" t="s">
         <v>19</v>
@@ -3710,16 +3725,16 @@
         <v>12</v>
       </c>
       <c r="R33" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="S33" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="T33" s="25" t="s">
+        <v>164</v>
+      </c>
+      <c r="U33" s="34" t="s">
         <v>156</v>
-      </c>
-      <c r="S33" s="25" t="s">
-        <v>157</v>
-      </c>
-      <c r="T33" s="25" t="s">
-        <v>167</v>
-      </c>
-      <c r="U33" s="34" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="34" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3738,7 +3753,7 @@
       <c r="E34" s="26"/>
       <c r="F34" s="35"/>
       <c r="G34" s="37" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="H34" s="27">
         <v>32</v>
@@ -3747,7 +3762,7 @@
         <v>92</v>
       </c>
       <c r="J34" s="38" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="K34" s="40" t="s">
         <v>69</v>
@@ -3767,16 +3782,16 @@
         <v>6</v>
       </c>
       <c r="R34" s="11" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="S34" s="11" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="T34" s="41" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="U34" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="35" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3795,7 +3810,7 @@
       <c r="E35" s="26"/>
       <c r="F35" s="35"/>
       <c r="G35" s="37" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="H35" s="27">
         <v>33</v>
@@ -3804,7 +3819,7 @@
         <v>92</v>
       </c>
       <c r="J35" s="38" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="K35" s="40" t="s">
         <v>69</v>
@@ -3847,7 +3862,7 @@
         <v>92</v>
       </c>
       <c r="J36" s="38" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="K36" s="40" t="s">
         <v>69</v>
@@ -3860,7 +3875,7 @@
         <v>23</v>
       </c>
       <c r="O36" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="P36" s="61" t="s">
         <v>19</v>
@@ -3869,16 +3884,16 @@
         <v>6</v>
       </c>
       <c r="R36" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="S36" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="T36" s="41" t="s">
+        <v>169</v>
+      </c>
+      <c r="U36" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="S36" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="T36" s="41" t="s">
-        <v>172</v>
-      </c>
-      <c r="U36" s="1" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
@@ -3897,7 +3912,7 @@
       <c r="E37" s="26"/>
       <c r="F37" s="35"/>
       <c r="G37" s="37" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="H37" s="27">
         <v>35</v>
@@ -3906,7 +3921,7 @@
         <v>92</v>
       </c>
       <c r="J37" s="38" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="K37" s="40" t="s">
         <v>69</v>
@@ -3926,16 +3941,16 @@
         <v>6</v>
       </c>
       <c r="R37" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="S37" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="T37" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="U37" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="S37" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="T37" s="41" t="s">
-        <v>197</v>
-      </c>
-      <c r="U37" s="1" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">

</xml_diff>